<commit_message>
Made changes to scripts to work on Mac
</commit_message>
<xml_diff>
--- a/Data/FalconTestData.xlsx
+++ b/Data/FalconTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niraj\PycharmProjects\RFTSeleniumTutorial\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhirrayapureddy/RFTFalcon/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8AE0B0-6B55-46AE-A594-D73A26BF6CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C58A68-30B5-5745-8C9F-B9E0C127B162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{D770CC2D-6A6F-458D-97EA-D55BC517FB0B}"/>
+    <workbookView xWindow="3440" yWindow="1180" windowWidth="21600" windowHeight="11380" xr2:uid="{D770CC2D-6A6F-458D-97EA-D55BC517FB0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bally" sheetId="1" r:id="rId1"/>
@@ -779,7 +779,7 @@
     <t>00</t>
   </si>
   <si>
-    <t>NEW-000683</t>
+    <t>NEW-000689</t>
   </si>
 </sst>
 </file>
@@ -2099,16 +2099,16 @@
   <dimension ref="A1:AP18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>224</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2268,12 +2268,12 @@
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -2283,7 +2283,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>198</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>215</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="11">
         <f>'[1]Step 1'!$E$9</f>
         <v>2300</v>
@@ -2723,16 +2723,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>239</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>240</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>241</v>
       </c>
@@ -2799,14 +2799,14 @@
       <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>22</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>37</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>38</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>Number of Years in Operation</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>39</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>&lt; 3 years (1.05-1.25)</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>40</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>=&lt;3 years and &lt;5 years (1.00-1.05)</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>41</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>42</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>43</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>44</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>45</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>46</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>47</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>48</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>49</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>50</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>51</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>52</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>53</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>Potential Cost &gt;3% of assets (1.20-1.30)</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>54</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>Potential Cost 1-3% of assets (1.10-1.20)</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>55</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>Potential Cost &lt;1% of assets (0.80-1.10)</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>56</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>57</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>58</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>0% (1)</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>59</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>60</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>61</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>62</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>63</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>64</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>65</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>35% (0.75-0.79)</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>66</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>40% (0.72-0.76)</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>67</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>68</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>69</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E53" s="24" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
@@ -4082,7 +4082,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E54" s="24" t="str">
         <f t="shared" si="1"/>
         <v>35%</v>
@@ -4103,7 +4103,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E55" s="24" t="str">
         <f t="shared" si="1"/>
         <v>40%</v>
@@ -4124,7 +4124,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E56" s="24" t="str">
         <f t="shared" si="1"/>
         <v>45%</v>
@@ -4142,7 +4142,7 @@
         <v>Comfortable (1)</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E57" s="24" t="str">
         <f t="shared" si="1"/>
         <v>50%</v>
@@ -4160,7 +4160,7 @@
         <v>Low Concern (1.00-1.15)</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F58" t="str">
         <f>'[2]Step 1'!$C$73</f>
         <v>Material Concern</v>
@@ -4174,7 +4174,7 @@
         <v>Material Concern (1.15-1.35)</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F59" t="str">
         <f>'[2]Step 1'!$C$74</f>
         <v>High Concern</v>
@@ -4188,7 +4188,7 @@
         <v>High Concern (1.35-1.75)</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F60" t="str">
         <f>'[2]Step 1'!$C$75</f>
         <v>Very High to Severe Concern</v>
@@ -4202,7 +4202,7 @@
         <v>Very High to Severe Concern (1.75-1.25)</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F62" t="s">
         <v>97</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>Discovery (Extended Reporting)</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F63" t="str">
         <f>'[2]Step 1'!$C$77</f>
         <v>1 year</v>
@@ -4228,7 +4228,7 @@
         <v>1 year (1)</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F64" t="str">
         <f>'[2]Step 1'!$C$78</f>
         <v>2 years</v>
@@ -4242,7 +4242,7 @@
         <v>2 years (175%-200%)</v>
       </c>
     </row>
-    <row r="65" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F65" t="str">
         <f>'[2]Step 1'!$C$79</f>
         <v>3 years</v>
@@ -4269,17 +4269,17 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="75.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="27">
         <v>1</v>
       </c>
@@ -4313,7 +4313,7 @@
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="27">
         <v>2</v>
       </c>
@@ -4347,7 +4347,7 @@
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="27">
         <v>3</v>
       </c>
@@ -4381,7 +4381,7 @@
       <c r="M3" s="27"/>
       <c r="N3" s="27"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="27">
         <v>4</v>
       </c>
@@ -4415,7 +4415,7 @@
       <c r="M4" s="27"/>
       <c r="N4" s="27"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="27">
         <v>5</v>
       </c>
@@ -4449,7 +4449,7 @@
       <c r="M5" s="27"/>
       <c r="N5" s="27"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="27">
         <v>6</v>
       </c>
@@ -4483,7 +4483,7 @@
       <c r="M6" s="27"/>
       <c r="N6" s="27"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="27">
         <v>7</v>
       </c>
@@ -4517,7 +4517,7 @@
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="27">
         <v>8</v>
       </c>
@@ -4551,7 +4551,7 @@
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="27">
         <v>9</v>
       </c>
@@ -4585,7 +4585,7 @@
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="27">
         <v>10</v>
       </c>
@@ -4619,7 +4619,7 @@
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="27">
         <v>11</v>
       </c>
@@ -4653,7 +4653,7 @@
       <c r="M11" s="27"/>
       <c r="N11" s="27"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="27">
         <v>12</v>
       </c>
@@ -4687,7 +4687,7 @@
       <c r="M12" s="27"/>
       <c r="N12" s="27"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="27">
         <v>13</v>
       </c>
@@ -4721,7 +4721,7 @@
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="27">
         <v>14</v>
       </c>
@@ -4755,7 +4755,7 @@
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="27">
         <v>15</v>
       </c>
@@ -4789,7 +4789,7 @@
       <c r="M15" s="27"/>
       <c r="N15" s="27"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="27">
         <v>16</v>
       </c>
@@ -4823,7 +4823,7 @@
       <c r="M16" s="27"/>
       <c r="N16" s="27"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="27">
         <v>17</v>
       </c>
@@ -4857,7 +4857,7 @@
       <c r="M17" s="27"/>
       <c r="N17" s="27"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="27">
         <v>18</v>
       </c>
@@ -4891,7 +4891,7 @@
       <c r="M18" s="27"/>
       <c r="N18" s="27"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="27">
         <v>19</v>
       </c>
@@ -4925,7 +4925,7 @@
       <c r="M19" s="27"/>
       <c r="N19" s="27"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="27">
         <v>20</v>
       </c>
@@ -4959,7 +4959,7 @@
       <c r="M20" s="27"/>
       <c r="N20" s="27"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="27">
         <v>21</v>
       </c>
@@ -4993,7 +4993,7 @@
       <c r="M21" s="27"/>
       <c r="N21" s="27"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="27">
         <v>22</v>
       </c>
@@ -5027,7 +5027,7 @@
       <c r="M22" s="27"/>
       <c r="N22" s="27"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="27">
         <v>23</v>
       </c>
@@ -5061,7 +5061,7 @@
       <c r="M23" s="27"/>
       <c r="N23" s="27"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
         <v>24</v>
       </c>
@@ -5095,7 +5095,7 @@
       <c r="M24" s="27"/>
       <c r="N24" s="27"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="27">
         <v>25</v>
       </c>
@@ -5129,7 +5129,7 @@
       <c r="M25" s="27"/>
       <c r="N25" s="27"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="27">
         <v>26</v>
       </c>
@@ -5163,7 +5163,7 @@
       <c r="M26" s="27"/>
       <c r="N26" s="27"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="27">
         <v>27</v>
       </c>
@@ -5197,7 +5197,7 @@
       <c r="M27" s="27"/>
       <c r="N27" s="27"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
         <v>28</v>
       </c>
@@ -5231,7 +5231,7 @@
       <c r="M28" s="27"/>
       <c r="N28" s="27"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="27">
         <v>29</v>
       </c>
@@ -5265,7 +5265,7 @@
       <c r="M29" s="27"/>
       <c r="N29" s="27"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="27">
         <v>30</v>
       </c>
@@ -5299,7 +5299,7 @@
       <c r="M30" s="27"/>
       <c r="N30" s="27"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -5315,7 +5315,7 @@
       <c r="M31" s="27"/>
       <c r="N31" s="27"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
@@ -5331,7 +5331,7 @@
       <c r="M32" s="27"/>
       <c r="N32" s="27"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="27"/>
       <c r="C33" s="27"/>
@@ -5347,7 +5347,7 @@
       <c r="M33" s="27"/>
       <c r="N33" s="27"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="27"/>
       <c r="B34" s="27"/>
       <c r="C34" s="27"/>

</xml_diff>

<commit_message>
Added Batch files to run Robot scripts
</commit_message>
<xml_diff>
--- a/Data/FalconTestData.xlsx
+++ b/Data/FalconTestData.xlsx
@@ -8,21 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niraj\PycharmProjects\RFTSeleniumTutorial\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D94DD44-3A60-4CB2-BA32-3E47E91A0CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D9B0ED-5683-4A84-B06E-65CB5C586309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1530" windowWidth="21600" windowHeight="11385" xr2:uid="{D770CC2D-6A6F-458D-97EA-D55BC517FB0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{D770CC2D-6A6F-458D-97EA-D55BC517FB0B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bally" sheetId="1" r:id="rId1"/>
-    <sheet name="Amazon" sheetId="6" r:id="rId2"/>
-    <sheet name="EnvLoginDetails" sheetId="5" r:id="rId3"/>
-    <sheet name="Data" sheetId="3" r:id="rId4"/>
-    <sheet name="UnderlyingPolicies" sheetId="4" r:id="rId5"/>
+    <sheet name="Amazon" sheetId="12" r:id="rId1"/>
+    <sheet name="Bally" sheetId="10" r:id="rId2"/>
+    <sheet name="Intel" sheetId="9" r:id="rId3"/>
+    <sheet name="Microsoft" sheetId="11" r:id="rId4"/>
+    <sheet name="UltaBeauty" sheetId="13" r:id="rId5"/>
+    <sheet name="EnvLoginDetails" sheetId="5" r:id="rId6"/>
+    <sheet name="Data" sheetId="3" r:id="rId7"/>
+    <sheet name="UnderlyingPolicies" sheetId="4" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,8 +49,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="255">
   <si>
     <t>testCase</t>
   </si>
@@ -760,9 +788,6 @@
     <t>Excess Follow form</t>
   </si>
   <si>
-    <t>BALY</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
@@ -772,22 +797,46 @@
     <t>NA_Falcon</t>
   </si>
   <si>
-    <t>HS Quote 1</t>
-  </si>
-  <si>
-    <t>NEW-000719</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
     <t>https://qa.oms.oneshield.com/Login</t>
   </si>
   <si>
     <t>QA</t>
   </si>
   <si>
-    <t>NEW-000695</t>
+    <t>00</t>
+  </si>
+  <si>
+    <t>Within 1 year (1.00-1.55)</t>
+  </si>
+  <si>
+    <t>Within 1-5 years (1.00-1.50)</t>
+  </si>
+  <si>
+    <t>25% (0.81-0.85)</t>
+  </si>
+  <si>
+    <t>Low Concern (1.00-1.15)</t>
+  </si>
+  <si>
+    <t>NEW-000698</t>
+  </si>
+  <si>
+    <t>Activity within 1-3 years / Material-high high concern (1.20-1.30)</t>
+  </si>
+  <si>
+    <t>&lt; 3 years (1.05-1.25)</t>
+  </si>
+  <si>
+    <t>Within 1 year (1.20-1.50)</t>
+  </si>
+  <si>
+    <t>Potential Cost 1-3% of assets (1.10-1.20)</t>
+  </si>
+  <si>
+    <t>10% (0.90-0.94)</t>
+  </si>
+  <si>
+    <t>Comfortable (1)</t>
   </si>
 </sst>
 </file>
@@ -799,16 +848,10 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1076,41 +1119,41 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="5" fontId="10" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="5" fontId="9" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -1127,24 +1170,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="6" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -1204,6 +1247,11 @@
             <v>Bally</v>
           </cell>
         </row>
+        <row r="8">
+          <cell r="E8" t="str">
+            <v>BALY</v>
+          </cell>
+        </row>
         <row r="9">
           <cell r="E9">
             <v>2300</v>
@@ -1234,11 +1282,6 @@
             <v>1</v>
           </cell>
         </row>
-        <row r="40">
-          <cell r="E40">
-            <v>0.95</v>
-          </cell>
-        </row>
         <row r="44">
           <cell r="E44">
             <v>1</v>
@@ -1256,7 +1299,7 @@
         </row>
         <row r="54">
           <cell r="E54">
-            <v>1</v>
+            <v>0.95</v>
           </cell>
         </row>
         <row r="56">
@@ -1264,11 +1307,6 @@
             <v>1</v>
           </cell>
         </row>
-        <row r="70">
-          <cell r="E70">
-            <v>0.9</v>
-          </cell>
-        </row>
         <row r="81">
           <cell r="E81">
             <v>1</v>
@@ -1380,8 +1418,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="16">
           <cell r="B16" t="str">
@@ -1389,25 +1427,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1483,11 +1521,6 @@
             <v>1</v>
           </cell>
         </row>
-        <row r="40">
-          <cell r="E40">
-            <v>0.95</v>
-          </cell>
-        </row>
         <row r="44">
           <cell r="E44">
             <v>1</v>
@@ -1513,11 +1546,6 @@
             <v>1</v>
           </cell>
         </row>
-        <row r="70">
-          <cell r="E70">
-            <v>0.9</v>
-          </cell>
-        </row>
         <row r="81">
           <cell r="E81">
             <v>1</v>
@@ -1616,6 +1644,484 @@
         <row r="100">
           <cell r="E100">
             <v>1</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="E101">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="E102">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>Public Organizations</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Step 1"/>
+      <sheetName val="Step 2"/>
+      <sheetName val="Step 3"/>
+      <sheetName val="XS Rating Step A Inputs"/>
+      <sheetName val="XS Rating Step B-F Inputs"/>
+      <sheetName val="XS Rating Step G Inputs"/>
+      <sheetName val="XS Final Premium Calculation"/>
+      <sheetName val="XS Final Premium Calculatio OLD"/>
+      <sheetName val="XS Rating Algorithm"/>
+      <sheetName val="XS Rating Algorithm OLD"/>
+      <sheetName val="XS Rate Tables Sections A-F"/>
+      <sheetName val="XS RateTables SectionA-Georgia"/>
+      <sheetName val="XS Rate Tables Section G"/>
+      <sheetName val="XS Rate Tables State Exceptions"/>
+      <sheetName val="Rating Plan Support --&gt;"/>
+      <sheetName val="Page 1"/>
+      <sheetName val="Page 2"/>
+      <sheetName val="ILF Interpolation"/>
+      <sheetName val="Curve Fitting"/>
+      <sheetName val="Extrapolation"/>
+      <sheetName val="Page 4"/>
+      <sheetName val="Page 5"/>
+      <sheetName val="Step 2a"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="7">
+          <cell r="E7" t="str">
+            <v>Ulta Beauty</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="E8" t="str">
+            <v>ULTA</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>19500</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="E10">
+            <v>5100</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>8100</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="E32">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="E33">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="E44">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="E48">
+            <v>0.8</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="E54">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="E56">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="E81">
+            <v>0.8</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="E82">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="E83">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="E84">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="E85">
+            <v>1.45</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="E86">
+            <v>1.1000000000000001</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="E87">
+            <v>1.26</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="E88">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="E89">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="E90">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="E91">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="E92">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="E93">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="E94">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="E95">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="E96">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="E97">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="E98">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="E99">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="E100">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="E101">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="E102">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>Public Organizations</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Step 1"/>
+      <sheetName val="Step 2"/>
+      <sheetName val="Step 3"/>
+      <sheetName val="XS Rating Step A Inputs"/>
+      <sheetName val="XS Rating Step B-F Inputs"/>
+      <sheetName val="XS Rating Step G Inputs"/>
+      <sheetName val="XS Final Premium Calculation"/>
+      <sheetName val="XS Final Premium Calculatio OLD"/>
+      <sheetName val="XS Rating Algorithm"/>
+      <sheetName val="XS Rating Algorithm OLD"/>
+      <sheetName val="XS Rate Tables Sections A-F"/>
+      <sheetName val="XS RateTables SectionA-Georgia"/>
+      <sheetName val="XS Rate Tables Section G"/>
+      <sheetName val="XS Rate Tables State Exceptions"/>
+      <sheetName val="Rating Plan Support --&gt;"/>
+      <sheetName val="Page 1"/>
+      <sheetName val="Page 2"/>
+      <sheetName val="ILF Interpolation"/>
+      <sheetName val="Curve Fitting"/>
+      <sheetName val="Extrapolation"/>
+      <sheetName val="Page 4"/>
+      <sheetName val="Page 5"/>
+      <sheetName val="Step 2a"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="7">
+          <cell r="E7" t="str">
+            <v>Intel</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="E8" t="str">
+            <v>INTC</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>188510</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="E10">
+            <v>168430</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>79020</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="E32">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="E33">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="E37">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="E41">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="E43">
+            <v>1.02</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="E52">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="E54">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="D77">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="D78" t="str">
+            <v>1.75-2.00</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="D79" t="str">
+            <v>2.25-2.50</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="E81">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="E82">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="E83">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="E84">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="E85">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="E86">
+            <v>1.1000000000000001</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="E87">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="E88">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="E89">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="E90">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="E91">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="E92">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="E93">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="E94">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="E95">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="E96">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="E97">
+            <v>0.8</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="E98">
+            <v>0.8</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="E99">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="E100">
+            <v>1.5</v>
           </cell>
         </row>
         <row r="101">
@@ -1634,7 +2140,7 @@
       <sheetData sheetId="3">
         <row r="16">
           <cell r="B16" t="str">
-            <v>Public Organizations</v>
+            <v>Private Organizations</v>
           </cell>
         </row>
       </sheetData>
@@ -1662,7 +2168,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1689,11 +2195,6 @@
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
-        <row r="32">
-          <cell r="B32" t="str">
-            <v>Credit for Side A Only with DIC Coverage</v>
-          </cell>
-        </row>
         <row r="35">
           <cell r="B35" t="str">
             <v>Number of Years in Operation</v>
@@ -1978,24 +2479,15 @@
           <cell r="C77" t="str">
             <v>1 year</v>
           </cell>
-          <cell r="D77">
-            <v>1</v>
-          </cell>
         </row>
         <row r="78">
           <cell r="C78" t="str">
             <v>2 years</v>
           </cell>
-          <cell r="D78" t="str">
-            <v>175%-200%</v>
-          </cell>
         </row>
         <row r="79">
           <cell r="C79" t="str">
             <v>3 years</v>
-          </cell>
-          <cell r="D79" t="str">
-            <v>225%-250%</v>
           </cell>
         </row>
       </sheetData>
@@ -2051,6 +2543,117 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Legend"/>
+      <sheetName val="Step 1"/>
+      <sheetName val="Step 2"/>
+      <sheetName val="Step 3"/>
+      <sheetName val="XS Rating Algorithm"/>
+      <sheetName val="XS Final Premium Calculation"/>
+      <sheetName val="XS Rate Tables Sections A-F"/>
+      <sheetName val="XS RateTables SectionA-Georgia"/>
+      <sheetName val="XS Rate Tables Section G"/>
+      <sheetName val="XS Rate Tables State Exceptions"/>
+      <sheetName val="XS Rating Step A Inputs"/>
+      <sheetName val="XS Rating Step B-F Inputs"/>
+      <sheetName val="XS Rating Step G Inputs"/>
+      <sheetName val="Rating Plan Support --&gt;"/>
+      <sheetName val="Page 1"/>
+      <sheetName val="Page 2"/>
+      <sheetName val="Page 4"/>
+      <sheetName val="Page 5"/>
+      <sheetName val="Step 2a"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="7">
+          <cell r="E7" t="str">
+            <v>Microsoft</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="E8" t="str">
+            <v>MSFT</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>109000</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="E10">
+            <v>125000</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>600000</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="E32">
+            <v>0.65</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="E33">
+            <v>0.55000000000000004</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="E37">
+            <v>1.05</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="E44">
+            <v>1.1000000000000001</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="E46">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="E54">
+            <v>0.95</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10">
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>Public Organizations</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2352,17 +2955,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C16D16E-3A0B-47E2-A40F-2732EB54521C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F49BE02-7912-44BD-A963-5393FFEC9B11}">
   <dimension ref="A1:AP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
@@ -2498,8 +3103,8 @@
         <v>224</v>
       </c>
       <c r="B2" t="str">
-        <f>'[1]Step 1'!$E$7</f>
-        <v>Bally</v>
+        <f>'[2]Step 1'!$E$7</f>
+        <v>Amazon</v>
       </c>
       <c r="C2" t="s">
         <v>226</v>
@@ -2519,10 +3124,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
@@ -2530,10 +3135,10 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D4" t="str">
         <f>IFERROR(VLOOKUP(C4,Data!$A:$B,2,FALSE)," ")</f>
@@ -2546,21 +3151,22 @@
       </c>
       <c r="B5" s="12">
         <f>B18*1000000</f>
-        <v>2300000000</v>
+        <v>1499722000000</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:D5" si="0">C18*1000000</f>
-        <v>1863000000</v>
+        <v>469820000000</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="0"/>
-        <v>961000000</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>238</v>
+        <v>33360000000</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f>'[2]Step 1'!$E$8</f>
+        <v>AMZN</v>
       </c>
       <c r="F5" s="13" t="str">
-        <f>'[1]XS Rating Step A Inputs'!$B$16</f>
+        <f>'[2]XS Rating Step A Inputs'!$B$16</f>
         <v>Public Organizations</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -2593,158 +3199,159 @@
         <v>101</v>
       </c>
       <c r="B6" s="15">
-        <f>'[1]Step 1'!$E$32</f>
+        <f>'[2]Step 1'!$E$32</f>
         <v>1</v>
       </c>
       <c r="C6" s="15">
-        <f>'[1]Step 1'!$E$33</f>
+        <f>'[2]Step 1'!$E$33</f>
         <v>1</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="15">
-        <f>'[1]Step 1'!$E$37</f>
+      <c r="E6" s="15" cm="1">
+        <f t="array" ref="E6">INDEX('[2]Step 1'!$E$35:'[2]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$35:'[2]Step 1'!$E$37),0))</f>
         <v>1</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="15">
-        <f>'[1]Step 1'!$E$40</f>
+      <c r="G6" s="15" cm="1">
+        <f t="array" ref="G6">INDEX('[2]Step 1'!$E$39:'[2]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$39:'[2]Step 1'!$E$41),0))</f>
         <v>0.95</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="I6" s="15">
-        <f>'[1]Step 1'!$E$44</f>
+        <v>244</v>
+      </c>
+      <c r="I6" s="15" cm="1">
+        <f t="array" ref="I6">INDEX('[2]Step 1'!$E$43:'[2]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$43:'[2]Step 1'!$E$44),0))</f>
         <v>1</v>
       </c>
       <c r="J6" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="15">
-        <f>'[1]Step 1'!$E$48</f>
+      <c r="K6" s="15" cm="1">
+        <f t="array" ref="K6">INDEX('[2]Step 1'!$E$46:'[2]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$46:'[2]Step 1'!$E$48),0))</f>
         <v>1</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="M6" s="15">
-        <f>'[1]Step 1'!$E$52</f>
+      <c r="M6" s="15" cm="1">
+        <f t="array" ref="M6">INDEX('[2]Step 1'!$E$50:'[2]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$50:'[2]Step 1'!$E$52),0))</f>
         <v>1</v>
       </c>
       <c r="N6" s="15">
-        <f>'[1]Step 1'!$E$54</f>
-        <v>1</v>
+        <f>'[2]Step 1'!$E$54</f>
+        <v>0.9</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="P6" s="15">
-        <f>'[1]Step 1'!$E$56</f>
+      <c r="P6" s="15" cm="1">
+        <f t="array" ref="P6">INDEX('[2]Step 1'!$E$56:'[2]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$56:'[2]Step 1'!$E$66),0))</f>
         <v>1</v>
       </c>
       <c r="Q6" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="R6" s="15">
-        <f>'[1]Step 1'!$E$70</f>
+      <c r="R6" s="15" cm="1">
+        <f t="array" ref="R6">INDEX('[2]Step 1'!$E$69:'[2]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$69:'[2]Step 1'!$E$75),0))</f>
         <v>0.9</v>
       </c>
       <c r="S6" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="T6" s="15">
+      <c r="T6" s="15" cm="1">
+        <f t="array" ref="T6">INDEX('[2]Step 1'!$E$77:'[2]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$77:'[2]Step 1'!$E$79),0))</f>
         <v>2</v>
       </c>
       <c r="U6" s="15">
-        <f>'[1]Step 1'!$E$81</f>
+        <f>'[2]Step 1'!$E$81</f>
         <v>1</v>
       </c>
       <c r="V6" s="15">
-        <f>'[1]Step 1'!$E$82</f>
+        <f>'[2]Step 1'!$E$82</f>
         <v>0.9</v>
       </c>
       <c r="W6" s="15">
-        <f>'[1]Step 1'!$E$83</f>
+        <f>'[2]Step 1'!$E$83</f>
         <v>1</v>
       </c>
       <c r="X6" s="15">
-        <f>'[1]Step 1'!$E$84</f>
+        <f>'[2]Step 1'!$E$84</f>
         <v>0.95</v>
       </c>
       <c r="Y6" s="15">
-        <f>'[1]Step 1'!$E$85</f>
+        <f>'[2]Step 1'!$E$85</f>
         <v>1</v>
       </c>
       <c r="Z6" s="15">
-        <f>'[1]Step 1'!$E$86</f>
+        <f>'[2]Step 1'!$E$86</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AA6" s="15">
-        <f>'[1]Step 1'!$E$87</f>
+        <f>'[2]Step 1'!$E$87</f>
         <v>1</v>
       </c>
       <c r="AB6" s="15">
-        <f>'[1]Step 1'!$E$88</f>
+        <f>'[2]Step 1'!$E$88</f>
         <v>1</v>
       </c>
       <c r="AC6" s="15">
-        <f>'[1]Step 1'!$E$89</f>
+        <f>'[2]Step 1'!$E$89</f>
         <v>1</v>
       </c>
       <c r="AD6" s="15">
-        <f>'[1]Step 1'!$E$90</f>
+        <f>'[2]Step 1'!$E$90</f>
         <v>0.95</v>
       </c>
       <c r="AE6" s="15">
-        <f>'[1]Step 1'!$E$91</f>
+        <f>'[2]Step 1'!$E$91</f>
         <v>0.95</v>
       </c>
       <c r="AF6" s="15">
-        <f>'[1]Step 1'!$E$92</f>
+        <f>'[2]Step 1'!$E$92</f>
         <v>0.9</v>
       </c>
       <c r="AG6" s="15">
-        <f>'[1]Step 1'!$E$93</f>
+        <f>'[2]Step 1'!$E$93</f>
         <v>0.95</v>
       </c>
       <c r="AH6" s="15">
-        <f>'[1]Step 1'!$E$94</f>
+        <f>'[2]Step 1'!$E$94</f>
         <v>1</v>
       </c>
       <c r="AI6" s="15">
-        <f>'[1]Step 1'!$E$95</f>
+        <f>'[2]Step 1'!$E$95</f>
         <v>1</v>
       </c>
       <c r="AJ6" s="15">
-        <f>'[1]Step 1'!$E$96</f>
+        <f>'[2]Step 1'!$E$96</f>
         <v>1</v>
       </c>
       <c r="AK6" s="15">
-        <f>'[1]Step 1'!$E$97</f>
+        <f>'[2]Step 1'!$E$97</f>
         <v>1</v>
       </c>
       <c r="AL6" s="15">
-        <f>'[1]Step 1'!$E$98</f>
+        <f>'[2]Step 1'!$E$98</f>
         <v>1</v>
       </c>
       <c r="AM6" s="15">
-        <f>'[1]Step 1'!$E$99</f>
+        <f>'[2]Step 1'!$E$99</f>
         <v>0.95</v>
       </c>
       <c r="AN6" s="15">
-        <f>'[1]Step 1'!$E$100</f>
+        <f>'[2]Step 1'!$E$100</f>
         <v>1</v>
       </c>
       <c r="AO6" s="15">
-        <f>'[1]Step 1'!$E$101</f>
+        <f>'[2]Step 1'!$E$101</f>
         <v>1</v>
       </c>
       <c r="AP6" s="15">
-        <f>'[1]Step 1'!$E$102</f>
+        <f>'[2]Step 1'!$E$102</f>
         <v>1</v>
       </c>
     </row>
@@ -2753,10 +3360,10 @@
         <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2845,122 +3452,747 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <f>'[1]Step 1'!$E$9</f>
-        <v>2300</v>
+        <f>'[2]Step 1'!$E$9</f>
+        <v>1499722</v>
       </c>
       <c r="C18" s="11">
-        <f>'[1]Step 1'!$E$10</f>
-        <v>1863</v>
+        <f>'[2]Step 1'!$E$10</f>
+        <v>469820</v>
       </c>
       <c r="D18" s="11">
-        <f>'[1]Step 1'!$E$11</f>
-        <v>961</v>
+        <f>'[2]Step 1'!$E$11</f>
+        <v>33360</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E3E778F-7F34-43C9-9EA2-BF8461C2163F}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{07BFD81D-2310-47A2-9E6F-14F08DB6A139}">
+          <x14:formula1>
+            <xm:f>Data!$U$25:$U$35</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{89603977-B441-48BD-9B49-14A8F786C4D6}">
+          <x14:formula1>
+            <xm:f>Data!$O$50:$O$55</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q8 S8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{01FECD05-AFC4-4F07-A56F-0742DF5EE565}">
+          <x14:formula1>
+            <xm:f>Data!$O$43:$O$47</xm:f>
+          </x14:formula1>
+          <xm:sqref>I8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AD99E27C-8AF1-4EC2-B21B-E5F6108251E9}">
+          <x14:formula1>
+            <xm:f>Data!$O$31:$O$35</xm:f>
+          </x14:formula1>
+          <xm:sqref>G8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{166638D9-FA68-45B0-A444-55EAEE12D7EC}">
+          <x14:formula1>
+            <xm:f>Data!$O$25:$O$27</xm:f>
+          </x14:formula1>
+          <xm:sqref>B8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6FFCB5C9-8A28-4B89-A0BB-FB3D6EC6CA78}">
+          <x14:formula1>
+            <xm:f>UnderlyingPolicies!$A$1:$A$30</xm:f>
+          </x14:formula1>
+          <xm:sqref>D7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6717E5E4-9C05-4B4E-ADA7-A02227939DEC}">
+          <x14:formula1>
+            <xm:f>Data!$H$63:$H$65</xm:f>
+          </x14:formula1>
+          <xm:sqref>S6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A5176B07-374C-4997-AB8C-6024A32FCC25}">
+          <x14:formula1>
+            <xm:f>Data!$H$54:$H$60</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{59B6A589-2BFA-4F29-80A7-9A455DE34B47}">
+          <x14:formula1>
+            <xm:f>Data!$H$41:$H$51</xm:f>
+          </x14:formula1>
+          <xm:sqref>O6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8A0F67F1-651C-4D77-A1E3-43D9AAB5CAEA}">
+          <x14:formula1>
+            <xm:f>Data!$H$36:$H$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>L6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C20FB9D2-278E-4BE0-A874-89D651730331}">
+          <x14:formula1>
+            <xm:f>Data!$H$31:$H$33</xm:f>
+          </x14:formula1>
+          <xm:sqref>J6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B66A281F-6C01-4B98-9396-23592EC33CA1}">
+          <x14:formula1>
+            <xm:f>Data!$H$27:$H$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>H6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{592E2A54-0A50-421D-872F-26240FB4700E}">
+          <x14:formula1>
+            <xm:f>Data!$H$17:$H$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>F6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FFF5A268-191A-4E5A-BC60-9B9CB8D9A90A}">
+          <x14:formula1>
+            <xm:f>Data!$H$22:$H$24</xm:f>
+          </x14:formula1>
+          <xm:sqref>D6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C05DF0FA-87E3-4CB8-8303-A4228C283160}">
+          <x14:formula1>
+            <xm:f>Data!$G$8:$G$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>H5:N5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AE8EA6F3-E5A7-4E61-9BFB-3E8A11F95ECB}">
+          <x14:formula1>
+            <xm:f>Data!$E$3:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G5 Y8 B7:C7 B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1907B1E0-C0DB-4CD4-A43C-45E06F38F2DB}">
           <x14:formula1>
             <xm:f>Data!$A$2:$A$52</xm:f>
           </x14:formula1>
           <xm:sqref>C4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C4D67323-05F0-4134-BA2D-EC09C999A885}">
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2091F9B8-959D-4870-A93A-0CB2DA15AFA9}">
+  <dimension ref="A1:AP18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" t="str">
+        <f>'[1]Step 1'!$E$7</f>
+        <v>Bally</v>
+      </c>
+      <c r="C2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="str">
+        <f>IFERROR(VLOOKUP(C4,Data!$A:$B,2,FALSE)," ")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="12">
+        <f>B18*1000000</f>
+        <v>2300000000</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" ref="C5:D5" si="0">C18*1000000</f>
+        <v>1863000000</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" si="0"/>
+        <v>961000000</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f>'[1]Step 1'!$E$8</f>
+        <v>BALY</v>
+      </c>
+      <c r="F5" s="13" t="str">
+        <f>'[1]XS Rating Step A Inputs'!$B$16</f>
+        <v>Public Organizations</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="15">
+        <f>'[1]Step 1'!$E$32</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="15">
+        <f>'[1]Step 1'!$E$33</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="15" cm="1">
+        <f t="array" ref="E6">INDEX('[1]Step 1'!$E$35:'[1]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$35:'[1]Step 1'!$E$37),0))</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" s="15" cm="1">
+        <f t="array" ref="G6">INDEX('[1]Step 1'!$E$39:'[1]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$39:'[1]Step 1'!$E$41),0))</f>
+        <v>0.95</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="15" cm="1">
+        <f t="array" ref="I6">INDEX('[1]Step 1'!$E$43:'[1]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$43:'[1]Step 1'!$E$44),0))</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="K6" s="15" cm="1">
+        <f t="array" ref="K6">INDEX('[1]Step 1'!$E$46:'[1]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$46:'[1]Step 1'!$E$48),0))</f>
+        <v>1</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6" s="15" cm="1">
+        <f t="array" ref="M6">INDEX('[1]Step 1'!$E$50:'[1]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$50:'[1]Step 1'!$E$52),0))</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="15">
+        <f>'[1]Step 1'!$E$54</f>
+        <v>0.95</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="P6" s="15" cm="1">
+        <f t="array" ref="P6">INDEX('[1]Step 1'!$E$56:'[1]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$56:'[1]Step 1'!$E$66),0))</f>
+        <v>1</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="R6" s="15" cm="1">
+        <f t="array" ref="R6">INDEX('[1]Step 1'!$E$69:'[1]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$69:'[1]Step 1'!$E$75),0))</f>
+        <v>0.9</v>
+      </c>
+      <c r="S6" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="T6" s="15" cm="1">
+        <f t="array" ref="T6">INDEX('[1]Step 1'!$E$77:'[1]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$77:'[1]Step 1'!$E$79),0))</f>
+        <v>2</v>
+      </c>
+      <c r="U6" s="15">
+        <f>'[1]Step 1'!$E$81</f>
+        <v>1</v>
+      </c>
+      <c r="V6" s="15">
+        <f>'[1]Step 1'!$E$82</f>
+        <v>0.9</v>
+      </c>
+      <c r="W6" s="15">
+        <f>'[1]Step 1'!$E$83</f>
+        <v>1</v>
+      </c>
+      <c r="X6" s="15">
+        <f>'[1]Step 1'!$E$84</f>
+        <v>0.95</v>
+      </c>
+      <c r="Y6" s="15">
+        <f>'[1]Step 1'!$E$85</f>
+        <v>1</v>
+      </c>
+      <c r="Z6" s="15">
+        <f>'[1]Step 1'!$E$86</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AA6" s="15">
+        <f>'[1]Step 1'!$E$87</f>
+        <v>1</v>
+      </c>
+      <c r="AB6" s="15">
+        <f>'[1]Step 1'!$E$88</f>
+        <v>1</v>
+      </c>
+      <c r="AC6" s="15">
+        <f>'[1]Step 1'!$E$89</f>
+        <v>1</v>
+      </c>
+      <c r="AD6" s="15">
+        <f>'[1]Step 1'!$E$90</f>
+        <v>0.95</v>
+      </c>
+      <c r="AE6" s="15">
+        <f>'[1]Step 1'!$E$91</f>
+        <v>0.95</v>
+      </c>
+      <c r="AF6" s="15">
+        <f>'[1]Step 1'!$E$92</f>
+        <v>0.9</v>
+      </c>
+      <c r="AG6" s="15">
+        <f>'[1]Step 1'!$E$93</f>
+        <v>0.95</v>
+      </c>
+      <c r="AH6" s="15">
+        <f>'[1]Step 1'!$E$94</f>
+        <v>1</v>
+      </c>
+      <c r="AI6" s="15">
+        <f>'[1]Step 1'!$E$95</f>
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="15">
+        <f>'[1]Step 1'!$E$96</f>
+        <v>1</v>
+      </c>
+      <c r="AK6" s="15">
+        <f>'[1]Step 1'!$E$97</f>
+        <v>1</v>
+      </c>
+      <c r="AL6" s="15">
+        <f>'[1]Step 1'!$E$98</f>
+        <v>1</v>
+      </c>
+      <c r="AM6" s="15">
+        <f>'[1]Step 1'!$E$99</f>
+        <v>0.95</v>
+      </c>
+      <c r="AN6" s="15">
+        <f>'[1]Step 1'!$E$100</f>
+        <v>1</v>
+      </c>
+      <c r="AO6" s="15">
+        <f>'[1]Step 1'!$E$101</f>
+        <v>1</v>
+      </c>
+      <c r="AP6" s="15">
+        <f>'[1]Step 1'!$E$102</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" t="str">
+        <f>D4</f>
+        <v>Yes</v>
+      </c>
+      <c r="G8" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8">
+        <v>45</v>
+      </c>
+      <c r="I8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J8">
+        <v>60</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>15</v>
+      </c>
+      <c r="P8">
+        <v>65</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>218</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>218</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>0.8</v>
+      </c>
+      <c r="W8">
+        <v>10</v>
+      </c>
+      <c r="X8">
+        <v>10</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA8">
+        <v>15000000</v>
+      </c>
+      <c r="AB8">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <f>'[1]Step 1'!$E$9</f>
+        <v>2300</v>
+      </c>
+      <c r="C18" s="11">
+        <f>'[1]Step 1'!$E$10</f>
+        <v>1863</v>
+      </c>
+      <c r="D18" s="11">
+        <f>'[1]Step 1'!$E$11</f>
+        <v>961</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6764BF2F-59F8-40E5-9C87-81F515C6E033}">
+          <x14:formula1>
+            <xm:f>Data!$A$2:$A$52</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA2DFE84-2FC1-4332-A94F-5622F5D20372}">
           <x14:formula1>
             <xm:f>Data!$E$3:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 G5 B7:C7 Y8</xm:sqref>
+          <xm:sqref>G5 Y8 B7:C7 B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5211930B-6801-49AA-97BD-BDA1CFAFEA62}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9171803-F478-4414-9387-09CCA3F55F54}">
           <x14:formula1>
             <xm:f>Data!$G$8:$G$12</xm:f>
           </x14:formula1>
           <xm:sqref>H5:N5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{91BC39E2-7F00-42CC-B0CA-8A8CC6D9D1F1}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FC15276D-FB91-4EBC-B0EE-DF7F674A84F0}">
           <x14:formula1>
             <xm:f>Data!$H$22:$H$24</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{52E38282-CB24-431C-B4D1-34A105A6FD65}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{232A58DB-028A-4C6D-B903-98AB845BD4CB}">
           <x14:formula1>
             <xm:f>Data!$H$17:$H$19</xm:f>
           </x14:formula1>
           <xm:sqref>F6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9D89A944-CAF1-47FE-86A7-3A056D6FAB07}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F2BB74BA-BF6A-4BC7-A052-E3203066F703}">
           <x14:formula1>
             <xm:f>Data!$H$27:$H$28</xm:f>
           </x14:formula1>
           <xm:sqref>H6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C67AB842-8B3F-43D5-962A-FEBCEEC7FE35}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AAC2379-0115-4BCA-9634-1AAD2BD9D87A}">
           <x14:formula1>
             <xm:f>Data!$H$31:$H$33</xm:f>
           </x14:formula1>
           <xm:sqref>J6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60131011-DB40-4889-B527-B3ABB5AB470D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C9A3696E-79DD-4340-9869-B95B5034322C}">
           <x14:formula1>
             <xm:f>Data!$H$36:$H$38</xm:f>
           </x14:formula1>
           <xm:sqref>L6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FF015303-FE86-4A19-846D-89DC99243564}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A393DF95-EC81-4662-A844-45EC0767314C}">
           <x14:formula1>
             <xm:f>Data!$H$41:$H$51</xm:f>
           </x14:formula1>
           <xm:sqref>O6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C4AE0C5-0D55-4584-A44D-9334AF5003B6}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D6517B3F-927D-4110-A49D-405879FB5489}">
           <x14:formula1>
             <xm:f>Data!$H$54:$H$60</xm:f>
           </x14:formula1>
           <xm:sqref>Q6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8286FA80-DD78-4CFC-9324-CDB26B17AE8C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3BC608E-52C5-47BE-9F9C-7217B7511BB4}">
           <x14:formula1>
             <xm:f>Data!$H$63:$H$65</xm:f>
           </x14:formula1>
           <xm:sqref>S6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A6583847-3BAE-4F3D-BD97-247E1181472E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8A547259-68EB-4679-AAC7-AD1C4D49B12D}">
           <x14:formula1>
             <xm:f>UnderlyingPolicies!$A$1:$A$30</xm:f>
           </x14:formula1>
           <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BF275A30-C3AD-46D9-A4DB-B0B83A385D9E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7499F666-6842-4404-89A7-D6A187741302}">
           <x14:formula1>
             <xm:f>Data!$O$25:$O$27</xm:f>
           </x14:formula1>
           <xm:sqref>B8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E07E7D5-1738-4EEB-B200-540476934E0D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BB325B27-5945-4F0A-8D23-1D106189003D}">
           <x14:formula1>
             <xm:f>Data!$O$31:$O$35</xm:f>
           </x14:formula1>
           <xm:sqref>G8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED54C5C3-7357-420B-BE1F-B0BE386C8FE0}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE7D1F4A-2EE3-4695-BD1C-AFE9771902E6}">
           <x14:formula1>
             <xm:f>Data!$O$43:$O$47</xm:f>
           </x14:formula1>
           <xm:sqref>I8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CBB0B3E5-B58F-4BBD-B330-9CE96F5197D3}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{115B5FEF-88B5-4D04-9ED6-164ACCA221E0}">
           <x14:formula1>
             <xm:f>Data!$O$50:$O$55</xm:f>
           </x14:formula1>
           <xm:sqref>Q8 S8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{967DAA2D-D6C9-4A2E-84E5-670248FAD53C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E645A3C-10C0-4D04-A3D9-0CD51DE5E707}">
           <x14:formula1>
             <xm:f>Data!$U$25:$U$35</xm:f>
           </x14:formula1>
@@ -2972,20 +4204,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB01EA3B-26C0-4304-BBF8-CA8FEB7AC308}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7431024C-B1CA-4198-BB91-2F4C2F294154}">
   <dimension ref="A1:AP18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
@@ -3121,8 +4353,8 @@
         <v>224</v>
       </c>
       <c r="B2" t="str">
-        <f>'[2]Step 1'!$E$7</f>
-        <v>Amazon</v>
+        <f>'[4]Step 1'!$E$7</f>
+        <v>Intel</v>
       </c>
       <c r="C2" t="s">
         <v>226</v>
@@ -3142,10 +4374,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
@@ -3156,11 +4388,11 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="D4" t="str">
         <f>IFERROR(VLOOKUP(C4,Data!$A:$B,2,FALSE)," ")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
@@ -3169,23 +4401,23 @@
       </c>
       <c r="B5" s="12">
         <f>B18*1000000</f>
-        <v>1499722000000</v>
+        <v>188510000000</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:D5" si="0">C18*1000000</f>
-        <v>469820000000</v>
+        <v>168430000000</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="0"/>
-        <v>33360000000</v>
+        <v>79020000000</v>
       </c>
       <c r="E5" s="13" t="str">
-        <f>'[2]Step 1'!$E$8</f>
-        <v>AMZN</v>
+        <f>'[4]Step 1'!$E$8</f>
+        <v>INTC</v>
       </c>
       <c r="F5" s="13" t="str">
-        <f>'[2]XS Rating Step A Inputs'!$B$16</f>
-        <v>Public Organizations</v>
+        <f>'[4]XS Rating Step A Inputs'!$B$16</f>
+        <v>Private Organizations</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>20</v>
@@ -3217,158 +4449,159 @@
         <v>101</v>
       </c>
       <c r="B6" s="15">
-        <f>'[2]Step 1'!$E$32</f>
+        <f>'[4]Step 1'!$E$32</f>
         <v>1</v>
       </c>
       <c r="C6" s="15">
-        <f>'[2]Step 1'!$E$33</f>
+        <f>'[4]Step 1'!$E$33</f>
         <v>1</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="15">
-        <f>'[2]Step 1'!$E$37</f>
-        <v>1</v>
+      <c r="E6" s="15" cm="1">
+        <f t="array" ref="E6">INDEX('[4]Step 1'!$E$35:'[4]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$35:'[4]Step 1'!$E$37),0))</f>
+        <v>0.9</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="15">
-        <f>'[2]Step 1'!$E$40</f>
-        <v>0.95</v>
+      <c r="G6" s="15" cm="1">
+        <f t="array" ref="G6">INDEX('[4]Step 1'!$E$39:'[4]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$39:'[4]Step 1'!$E$41),0))</f>
+        <v>1</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="I6" s="15">
-        <f>'[2]Step 1'!$E$44</f>
-        <v>1</v>
+        <v>244</v>
+      </c>
+      <c r="I6" s="15" cm="1">
+        <f t="array" ref="I6">INDEX('[4]Step 1'!$E$43:'[4]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$43:'[4]Step 1'!$E$44),0))</f>
+        <v>1.02</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="K6" s="15">
-        <f>'[2]Step 1'!$E$48</f>
-        <v>1</v>
+        <v>245</v>
+      </c>
+      <c r="K6" s="15" cm="1">
+        <f t="array" ref="K6">INDEX('[4]Step 1'!$E$46:'[4]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$46:'[4]Step 1'!$E$48),0))</f>
+        <v>1.36</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="M6" s="15">
-        <f>'[2]Step 1'!$E$52</f>
-        <v>1</v>
+      <c r="M6" s="15" cm="1">
+        <f t="array" ref="M6">INDEX('[4]Step 1'!$E$50:'[4]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$50:'[4]Step 1'!$E$52),0))</f>
+        <v>0.95</v>
       </c>
       <c r="N6" s="15">
-        <f>'[2]Step 1'!$E$54</f>
-        <v>0.9</v>
+        <f>'[4]Step 1'!$E$54</f>
+        <v>1</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="P6" s="15">
-        <f>'[2]Step 1'!$E$56</f>
-        <v>1</v>
+        <v>246</v>
+      </c>
+      <c r="P6" s="15" cm="1">
+        <f t="array" ref="P6">INDEX('[4]Step 1'!$E$56:'[4]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$56:'[4]Step 1'!$E$66),0))</f>
+        <v>0.81</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="R6" s="15">
-        <f>'[2]Step 1'!$E$70</f>
-        <v>0.9</v>
+        <v>247</v>
+      </c>
+      <c r="R6" s="15" cm="1">
+        <f t="array" ref="R6">INDEX('[4]Step 1'!$E$69:'[4]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$69:'[4]Step 1'!$E$75),0))</f>
+        <v>1.05</v>
       </c>
       <c r="S6" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="T6" s="15">
+      <c r="T6" s="15" cm="1">
+        <f t="array" ref="T6">INDEX('[4]Step 1'!$E$77:'[4]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$77:'[4]Step 1'!$E$79),0))</f>
         <v>2</v>
       </c>
       <c r="U6" s="15">
-        <f>'[2]Step 1'!$E$81</f>
+        <f>'[4]Step 1'!$E$81</f>
         <v>1</v>
       </c>
       <c r="V6" s="15">
-        <f>'[2]Step 1'!$E$82</f>
+        <f>'[4]Step 1'!$E$82</f>
         <v>0.9</v>
       </c>
       <c r="W6" s="15">
-        <f>'[2]Step 1'!$E$83</f>
+        <f>'[4]Step 1'!$E$83</f>
         <v>1</v>
       </c>
       <c r="X6" s="15">
-        <f>'[2]Step 1'!$E$84</f>
+        <f>'[4]Step 1'!$E$84</f>
         <v>0.95</v>
       </c>
       <c r="Y6" s="15">
-        <f>'[2]Step 1'!$E$85</f>
+        <f>'[4]Step 1'!$E$85</f>
         <v>1</v>
       </c>
       <c r="Z6" s="15">
-        <f>'[2]Step 1'!$E$86</f>
+        <f>'[4]Step 1'!$E$86</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AA6" s="15">
-        <f>'[2]Step 1'!$E$87</f>
+        <f>'[4]Step 1'!$E$87</f>
         <v>1</v>
       </c>
       <c r="AB6" s="15">
-        <f>'[2]Step 1'!$E$88</f>
+        <f>'[4]Step 1'!$E$88</f>
         <v>1</v>
       </c>
       <c r="AC6" s="15">
-        <f>'[2]Step 1'!$E$89</f>
+        <f>'[4]Step 1'!$E$89</f>
         <v>1</v>
       </c>
       <c r="AD6" s="15">
-        <f>'[2]Step 1'!$E$90</f>
+        <f>'[4]Step 1'!$E$90</f>
         <v>0.95</v>
       </c>
       <c r="AE6" s="15">
-        <f>'[2]Step 1'!$E$91</f>
+        <f>'[4]Step 1'!$E$91</f>
         <v>0.95</v>
       </c>
       <c r="AF6" s="15">
-        <f>'[2]Step 1'!$E$92</f>
+        <f>'[4]Step 1'!$E$92</f>
         <v>0.9</v>
       </c>
       <c r="AG6" s="15">
-        <f>'[2]Step 1'!$E$93</f>
+        <f>'[4]Step 1'!$E$93</f>
         <v>0.95</v>
       </c>
       <c r="AH6" s="15">
-        <f>'[2]Step 1'!$E$94</f>
+        <f>'[4]Step 1'!$E$94</f>
         <v>1</v>
       </c>
       <c r="AI6" s="15">
-        <f>'[2]Step 1'!$E$95</f>
+        <f>'[4]Step 1'!$E$95</f>
         <v>1</v>
       </c>
       <c r="AJ6" s="15">
-        <f>'[2]Step 1'!$E$96</f>
+        <f>'[4]Step 1'!$E$96</f>
         <v>1</v>
       </c>
       <c r="AK6" s="15">
-        <f>'[2]Step 1'!$E$97</f>
-        <v>1</v>
+        <f>'[4]Step 1'!$E$97</f>
+        <v>0.8</v>
       </c>
       <c r="AL6" s="15">
-        <f>'[2]Step 1'!$E$98</f>
-        <v>1</v>
+        <f>'[4]Step 1'!$E$98</f>
+        <v>0.8</v>
       </c>
       <c r="AM6" s="15">
-        <f>'[2]Step 1'!$E$99</f>
+        <f>'[4]Step 1'!$E$99</f>
         <v>0.95</v>
       </c>
       <c r="AN6" s="15">
-        <f>'[2]Step 1'!$E$100</f>
-        <v>1</v>
+        <f>'[4]Step 1'!$E$100</f>
+        <v>1.5</v>
       </c>
       <c r="AO6" s="15">
-        <f>'[2]Step 1'!$E$101</f>
+        <f>'[4]Step 1'!$E$101</f>
         <v>1</v>
       </c>
       <c r="AP6" s="15">
-        <f>'[2]Step 1'!$E$102</f>
+        <f>'[4]Step 1'!$E$102</f>
         <v>1</v>
       </c>
     </row>
@@ -3377,10 +4610,10 @@
         <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -3394,7 +4627,7 @@
         <v>201</v>
       </c>
       <c r="C8" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -3404,7 +4637,7 @@
       </c>
       <c r="F8" t="str">
         <f>D4</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G8" t="s">
         <v>205</v>
@@ -3413,10 +4646,10 @@
         <v>45</v>
       </c>
       <c r="I8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J8">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="K8">
         <v>5</v>
@@ -3469,121 +4702,122 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <f>'[2]Step 1'!$E$9</f>
-        <v>1499722</v>
+        <f>'[4]Step 1'!$E$9</f>
+        <v>188510</v>
       </c>
       <c r="C18" s="11">
-        <f>'[2]Step 1'!$E$10</f>
-        <v>469820</v>
+        <f>'[4]Step 1'!$E$10</f>
+        <v>168430</v>
       </c>
       <c r="D18" s="11">
-        <f>'[2]Step 1'!$E$11</f>
-        <v>33360</v>
+        <f>'[4]Step 1'!$E$11</f>
+        <v>79020</v>
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F42E000C-7831-4562-86AF-B26FA7F3A5BD}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60EBAD5C-6228-45A6-8B40-D5BFA17D4FFB}">
           <x14:formula1>
             <xm:f>Data!$U$25:$U$35</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5AB87932-5F18-4DB8-A910-C21520A8F278}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E669DA6-8732-4DFC-BB3F-4E0D9298CDD0}">
           <x14:formula1>
             <xm:f>Data!$O$50:$O$55</xm:f>
           </x14:formula1>
           <xm:sqref>Q8 S8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7B50B160-2E48-47F1-8752-DAC671030DC2}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D20C171B-16BF-4799-B26C-A500DB35BF11}">
           <x14:formula1>
             <xm:f>Data!$O$43:$O$47</xm:f>
           </x14:formula1>
           <xm:sqref>I8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C2766560-F3D3-4A1E-85C1-1802DEBC649C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4838A53F-8E91-4E5F-9F30-3A3E2C630E40}">
           <x14:formula1>
             <xm:f>Data!$O$31:$O$35</xm:f>
           </x14:formula1>
           <xm:sqref>G8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{15B90E77-1B3D-4CB7-815C-9F2C7CC90CB6}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{03FC0A59-C08F-41AE-A940-191C1E7C6CA7}">
           <x14:formula1>
             <xm:f>Data!$O$25:$O$27</xm:f>
           </x14:formula1>
           <xm:sqref>B8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{85C915DF-03AE-413C-8D2F-B8F5638E0CC9}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5274FDC8-D4F8-4EEB-A852-AD5D5179A52E}">
           <x14:formula1>
             <xm:f>UnderlyingPolicies!$A$1:$A$30</xm:f>
           </x14:formula1>
           <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA80C557-7B2B-46D6-B25C-EF6A7F239650}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EAF97C30-032F-4363-ABE9-CBC9E0CF8766}">
           <x14:formula1>
             <xm:f>Data!$H$63:$H$65</xm:f>
           </x14:formula1>
           <xm:sqref>S6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0069BA3F-7CCB-4433-82BA-37298C738A94}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2F55E8D7-9398-4EA3-9CCC-27ACDA95C21B}">
           <x14:formula1>
             <xm:f>Data!$H$54:$H$60</xm:f>
           </x14:formula1>
           <xm:sqref>Q6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA9CD727-6850-4048-9729-73AFAA22AEBA}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FD842F6-8F5A-440B-BC48-7D5820A3F6DE}">
           <x14:formula1>
             <xm:f>Data!$H$41:$H$51</xm:f>
           </x14:formula1>
           <xm:sqref>O6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3D77B846-4EC6-45B1-9CE3-E82EFC010519}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B868AF8F-49BF-4CA3-83BB-4894BA65EC6B}">
           <x14:formula1>
             <xm:f>Data!$H$36:$H$38</xm:f>
           </x14:formula1>
           <xm:sqref>L6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D905603D-493F-4065-8F91-D788B4BCD080}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3146C091-F835-4D5A-B1D6-49B4F9D41842}">
           <x14:formula1>
             <xm:f>Data!$H$31:$H$33</xm:f>
           </x14:formula1>
           <xm:sqref>J6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C51ACDDB-F947-4A94-BAEA-D2527014D0FB}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B35C1E48-73C0-4426-8E84-E2B417121F86}">
           <x14:formula1>
             <xm:f>Data!$H$27:$H$28</xm:f>
           </x14:formula1>
           <xm:sqref>H6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5E5EC81A-962C-43EF-9553-BCD65F2C305E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7F1B1D07-751E-4A38-A665-265A595428D4}">
           <x14:formula1>
             <xm:f>Data!$H$17:$H$19</xm:f>
           </x14:formula1>
           <xm:sqref>F6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6C2EB40E-D551-417A-A979-20F58128B0DA}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5705444F-F4C7-4F7E-A410-466DA7AC6EF8}">
           <x14:formula1>
             <xm:f>Data!$H$22:$H$24</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB9CE9C6-E492-400B-96CD-4DAB962A24EA}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BF2722E-295C-459C-A4C3-CB4DB28E4645}">
           <x14:formula1>
             <xm:f>Data!$G$8:$G$12</xm:f>
           </x14:formula1>
           <xm:sqref>H5:N5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B6357FAC-2C26-420D-817A-5C953A81FD55}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7B0043AE-B4E5-43AA-9F9E-E6A09E977C57}">
           <x14:formula1>
             <xm:f>Data!$E$3:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 G5 B7:C7 Y8</xm:sqref>
+          <xm:sqref>G5 Y8 B7:C7 B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{14EAD095-5B2E-4D1C-B113-68EC3F95F830}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0F1571A5-F984-469D-81EA-105E3E40627D}">
           <x14:formula1>
             <xm:f>Data!$A$2:$A$52</xm:f>
           </x14:formula1>
@@ -3595,7 +4829,1257 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F17AA2-79AB-407C-84B8-5B195D81098D}">
+  <dimension ref="A1:AP18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" t="str">
+        <f>'[6]Step 1'!$E$7</f>
+        <v>Microsoft</v>
+      </c>
+      <c r="C2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="str">
+        <f>IFERROR(VLOOKUP(C4,Data!$A:$B,2,FALSE)," ")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="12">
+        <f>B18*1000000</f>
+        <v>109000000000</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" ref="C5:D5" si="0">C18*1000000</f>
+        <v>125000000000</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" si="0"/>
+        <v>600000000000</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f>'[6]Step 1'!$E$8</f>
+        <v>MSFT</v>
+      </c>
+      <c r="F5" s="13" t="str">
+        <f>'[6]XS Rating Step A Inputs'!$B$16</f>
+        <v>Public Organizations</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="15">
+        <f>'[6]Step 1'!$E$32</f>
+        <v>0.65</v>
+      </c>
+      <c r="C6" s="15">
+        <f>'[6]Step 1'!$E$33</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="E6" s="15" cm="1">
+        <f t="array" ref="E6">INDEX('[6]Step 1'!$E$35:'[6]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$35:'[6]Step 1'!$E$37),0))</f>
+        <v>1.05</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" s="15" cm="1">
+        <f t="array" ref="G6">INDEX('[6]Step 1'!$E$39:'[6]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$39:'[6]Step 1'!$E$41),0))</f>
+        <v>1.25</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="15" cm="1">
+        <f t="array" ref="I6">INDEX('[6]Step 1'!$E$43:'[6]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$43:'[6]Step 1'!$E$44),0))</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="K6" s="15" cm="1">
+        <f t="array" ref="K6">INDEX('[6]Step 1'!$E$46:'[6]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$46:'[6]Step 1'!$E$48),0))</f>
+        <v>1.2</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="M6" s="15" cm="1">
+        <f t="array" ref="M6">INDEX('[6]Step 1'!$E$50:'[6]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$50:'[6]Step 1'!$E$52),0))</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N6" s="15">
+        <f>'[6]Step 1'!$E$54</f>
+        <v>0.95</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="P6" s="15" cm="1">
+        <f t="array" ref="P6">INDEX('[6]Step 1'!$E$56:'[6]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$56:'[6]Step 1'!$E$66),0))</f>
+        <v>0.93</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="R6" s="15" cm="1">
+        <f t="array" ref="R6">INDEX('[6]Step 1'!$E$69:'[6]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$69:'[6]Step 1'!$E$75),0))</f>
+        <v>1</v>
+      </c>
+      <c r="S6" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="T6" s="15" cm="1">
+        <f t="array" ref="T6">INDEX('[6]Step 1'!$E$77:'[6]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$77:'[6]Step 1'!$E$79),0))</f>
+        <v>1.75</v>
+      </c>
+      <c r="U6" s="15">
+        <f>'[6]Step 1'!$E$81</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="15">
+        <f>'[6]Step 1'!$E$82</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="15">
+        <f>'[6]Step 1'!$E$83</f>
+        <v>0</v>
+      </c>
+      <c r="X6" s="15">
+        <f>'[6]Step 1'!$E$84</f>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="15">
+        <f>'[6]Step 1'!$E$85</f>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="15">
+        <f>'[6]Step 1'!$E$86</f>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="15">
+        <f>'[6]Step 1'!$E$87</f>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="15">
+        <f>'[6]Step 1'!$E$88</f>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="15">
+        <f>'[6]Step 1'!$E$89</f>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="15">
+        <f>'[6]Step 1'!$E$90</f>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="15">
+        <f>'[6]Step 1'!$E$91</f>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="15">
+        <f>'[6]Step 1'!$E$92</f>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="15">
+        <f>'[6]Step 1'!$E$93</f>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="15">
+        <f>'[6]Step 1'!$E$94</f>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="15">
+        <f>'[6]Step 1'!$E$95</f>
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="15">
+        <f>'[6]Step 1'!$E$96</f>
+        <v>0</v>
+      </c>
+      <c r="AK6" s="15">
+        <f>'[6]Step 1'!$E$97</f>
+        <v>0</v>
+      </c>
+      <c r="AL6" s="15">
+        <f>'[6]Step 1'!$E$98</f>
+        <v>0</v>
+      </c>
+      <c r="AM6" s="15">
+        <f>'[6]Step 1'!$E$99</f>
+        <v>0</v>
+      </c>
+      <c r="AN6" s="15">
+        <f>'[6]Step 1'!$E$100</f>
+        <v>0</v>
+      </c>
+      <c r="AO6" s="15">
+        <f>'[6]Step 1'!$E$101</f>
+        <v>0</v>
+      </c>
+      <c r="AP6" s="15">
+        <f>'[6]Step 1'!$E$102</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" t="str">
+        <f>D4</f>
+        <v>Yes</v>
+      </c>
+      <c r="G8" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8">
+        <v>45</v>
+      </c>
+      <c r="I8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J8">
+        <v>60</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>15</v>
+      </c>
+      <c r="P8">
+        <v>65</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>218</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>218</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>0.8</v>
+      </c>
+      <c r="W8">
+        <v>10</v>
+      </c>
+      <c r="X8">
+        <v>10</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA8">
+        <v>15000000</v>
+      </c>
+      <c r="AB8">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <f>'[6]Step 1'!$E$9</f>
+        <v>109000</v>
+      </c>
+      <c r="C18" s="11">
+        <f>'[6]Step 1'!$E$10</f>
+        <v>125000</v>
+      </c>
+      <c r="D18" s="11">
+        <f>'[6]Step 1'!$E$11</f>
+        <v>600000</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BB914539-CF63-490D-9726-61DE3D777103}">
+          <x14:formula1>
+            <xm:f>Data!$U$25:$U$35</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CBC411BD-3B7C-4094-888E-E018F9E257BA}">
+          <x14:formula1>
+            <xm:f>Data!$O$50:$O$55</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q8 S8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A2D20CE8-4927-4F47-8400-26B13B3A8458}">
+          <x14:formula1>
+            <xm:f>Data!$O$43:$O$47</xm:f>
+          </x14:formula1>
+          <xm:sqref>I8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C2218858-166E-4C09-BC2F-16E74AC961A4}">
+          <x14:formula1>
+            <xm:f>Data!$O$31:$O$35</xm:f>
+          </x14:formula1>
+          <xm:sqref>G8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7882F147-E08C-4BF8-AAD9-C616E71C6310}">
+          <x14:formula1>
+            <xm:f>Data!$O$25:$O$27</xm:f>
+          </x14:formula1>
+          <xm:sqref>B8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{905CCF32-07B0-46E3-98F1-76677166BF70}">
+          <x14:formula1>
+            <xm:f>UnderlyingPolicies!$A$1:$A$30</xm:f>
+          </x14:formula1>
+          <xm:sqref>D7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E136F28D-EFC7-4636-BB41-D9BE47E38561}">
+          <x14:formula1>
+            <xm:f>Data!$H$63:$H$65</xm:f>
+          </x14:formula1>
+          <xm:sqref>S6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{63608154-4AD8-46CF-B172-3936800C5478}">
+          <x14:formula1>
+            <xm:f>Data!$H$54:$H$60</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ADFBD46D-54BF-4631-812D-83114D02ED20}">
+          <x14:formula1>
+            <xm:f>Data!$H$41:$H$51</xm:f>
+          </x14:formula1>
+          <xm:sqref>O6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{756A1990-8866-464B-8BB6-A4A99A2CC823}">
+          <x14:formula1>
+            <xm:f>Data!$H$36:$H$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>L6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{797D976C-3054-4FCF-888B-CC771DAAD0DD}">
+          <x14:formula1>
+            <xm:f>Data!$H$31:$H$33</xm:f>
+          </x14:formula1>
+          <xm:sqref>J6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3BAFCF94-CC53-442A-84F7-D231F387A984}">
+          <x14:formula1>
+            <xm:f>Data!$H$27:$H$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>H6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DB68DC3E-B9AA-4B89-B33C-EDD17B4A6337}">
+          <x14:formula1>
+            <xm:f>Data!$H$17:$H$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>F6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D82BA4E6-1442-4FCE-8C96-6146658F1045}">
+          <x14:formula1>
+            <xm:f>Data!$H$22:$H$24</xm:f>
+          </x14:formula1>
+          <xm:sqref>D6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{07FD1E50-7CFE-4733-9E97-FDC49F33EAA9}">
+          <x14:formula1>
+            <xm:f>Data!$G$8:$G$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>H5:N5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{88FE88FB-60C8-4FF2-95FA-B98129E06643}">
+          <x14:formula1>
+            <xm:f>Data!$E$3:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G5 Y8 B7:C7 B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{24CD61D0-4ADB-4B69-AD6F-D74DF5C1F11F}">
+          <x14:formula1>
+            <xm:f>Data!$A$2:$A$52</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515B94FA-5A74-4B2F-AE46-2F448621C2E3}">
+  <dimension ref="A1:AP18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" t="str">
+        <f>'[3]Step 1'!$E$7</f>
+        <v>Ulta Beauty</v>
+      </c>
+      <c r="C2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="str">
+        <f>IFERROR(VLOOKUP(C4,Data!$A:$B,2,FALSE)," ")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="12">
+        <f>B18*1000000</f>
+        <v>19500000000</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" ref="C5:D5" si="0">C18*1000000</f>
+        <v>5100000000</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" si="0"/>
+        <v>8100000000</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f>'[3]Step 1'!$E$8</f>
+        <v>ULTA</v>
+      </c>
+      <c r="F5" s="13" t="str">
+        <f>'[3]XS Rating Step A Inputs'!$B$16</f>
+        <v>Public Organizations</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="15">
+        <f>'[3]Step 1'!$E$32</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="15">
+        <f>'[3]Step 1'!$E$33</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="15" cm="1">
+        <f t="array" ref="E6">INDEX('[3]Step 1'!$E$35:'[3]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$35:'[3]Step 1'!$E$37),0))</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="15" cm="1">
+        <f t="array" ref="G6">INDEX('[3]Step 1'!$E$39:'[3]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$39:'[3]Step 1'!$E$41),0))</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="I6" s="15" cm="1">
+        <f t="array" ref="I6">INDEX('[3]Step 1'!$E$43:'[3]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$43:'[3]Step 1'!$E$44),0))</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="K6" s="15" cm="1">
+        <f t="array" ref="K6">INDEX('[3]Step 1'!$E$46:'[3]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$46:'[3]Step 1'!$E$48),0))</f>
+        <v>0.8</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6" s="15" cm="1">
+        <f t="array" ref="M6">INDEX('[3]Step 1'!$E$50:'[3]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$50:'[3]Step 1'!$E$52),0))</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="15">
+        <f>'[3]Step 1'!$E$54</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="P6" s="15" cm="1">
+        <f t="array" ref="P6">INDEX('[3]Step 1'!$E$56:'[3]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$56:'[3]Step 1'!$E$66),0))</f>
+        <v>1</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="R6" s="15" cm="1">
+        <f t="array" ref="R6">INDEX('[3]Step 1'!$E$69:'[3]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$69:'[3]Step 1'!$E$75),0))</f>
+        <v>0.9</v>
+      </c>
+      <c r="S6" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="T6" s="15" cm="1">
+        <f t="array" ref="T6">INDEX('[3]Step 1'!$E$77:'[3]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$77:'[3]Step 1'!$E$79),0))</f>
+        <v>2</v>
+      </c>
+      <c r="U6" s="15">
+        <f>'[3]Step 1'!$E$81</f>
+        <v>0.8</v>
+      </c>
+      <c r="V6" s="15">
+        <f>'[3]Step 1'!$E$82</f>
+        <v>0.9</v>
+      </c>
+      <c r="W6" s="15">
+        <f>'[3]Step 1'!$E$83</f>
+        <v>1</v>
+      </c>
+      <c r="X6" s="15">
+        <f>'[3]Step 1'!$E$84</f>
+        <v>0.95</v>
+      </c>
+      <c r="Y6" s="15">
+        <f>'[3]Step 1'!$E$85</f>
+        <v>1.45</v>
+      </c>
+      <c r="Z6" s="15">
+        <f>'[3]Step 1'!$E$86</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AA6" s="15">
+        <f>'[3]Step 1'!$E$87</f>
+        <v>1.26</v>
+      </c>
+      <c r="AB6" s="15">
+        <f>'[3]Step 1'!$E$88</f>
+        <v>1</v>
+      </c>
+      <c r="AC6" s="15">
+        <f>'[3]Step 1'!$E$89</f>
+        <v>1</v>
+      </c>
+      <c r="AD6" s="15">
+        <f>'[3]Step 1'!$E$90</f>
+        <v>0.95</v>
+      </c>
+      <c r="AE6" s="15">
+        <f>'[3]Step 1'!$E$91</f>
+        <v>0.95</v>
+      </c>
+      <c r="AF6" s="15">
+        <f>'[3]Step 1'!$E$92</f>
+        <v>0.9</v>
+      </c>
+      <c r="AG6" s="15">
+        <f>'[3]Step 1'!$E$93</f>
+        <v>1</v>
+      </c>
+      <c r="AH6" s="15">
+        <f>'[3]Step 1'!$E$94</f>
+        <v>1</v>
+      </c>
+      <c r="AI6" s="15">
+        <f>'[3]Step 1'!$E$95</f>
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="15">
+        <f>'[3]Step 1'!$E$96</f>
+        <v>1</v>
+      </c>
+      <c r="AK6" s="15">
+        <f>'[3]Step 1'!$E$97</f>
+        <v>1</v>
+      </c>
+      <c r="AL6" s="15">
+        <f>'[3]Step 1'!$E$98</f>
+        <v>1</v>
+      </c>
+      <c r="AM6" s="15">
+        <f>'[3]Step 1'!$E$99</f>
+        <v>0.95</v>
+      </c>
+      <c r="AN6" s="15">
+        <f>'[3]Step 1'!$E$100</f>
+        <v>1</v>
+      </c>
+      <c r="AO6" s="15">
+        <f>'[3]Step 1'!$E$101</f>
+        <v>1</v>
+      </c>
+      <c r="AP6" s="15">
+        <f>'[3]Step 1'!$E$102</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" t="str">
+        <f>D4</f>
+        <v>Yes</v>
+      </c>
+      <c r="G8" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8">
+        <v>45</v>
+      </c>
+      <c r="I8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J8">
+        <v>60</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>15</v>
+      </c>
+      <c r="P8">
+        <v>65</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>218</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>218</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>0.8</v>
+      </c>
+      <c r="W8">
+        <v>10</v>
+      </c>
+      <c r="X8">
+        <v>10</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA8">
+        <v>15000000</v>
+      </c>
+      <c r="AB8">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <f>'[3]Step 1'!$E$9</f>
+        <v>19500</v>
+      </c>
+      <c r="C18" s="11">
+        <f>'[3]Step 1'!$E$10</f>
+        <v>5100</v>
+      </c>
+      <c r="D18" s="11">
+        <f>'[3]Step 1'!$E$11</f>
+        <v>8100</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A77D1720-C05C-4574-915B-04461B72A85E}">
+          <x14:formula1>
+            <xm:f>Data!$A$2:$A$52</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C9EE6B70-D4C2-42AA-A96F-DC20B6C3A6D3}">
+          <x14:formula1>
+            <xm:f>Data!$E$3:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G5 Y8 B7:C7 B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7EAF63FC-F364-47A1-B3A0-F5EC426E6B74}">
+          <x14:formula1>
+            <xm:f>Data!$G$8:$G$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>H5:N5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{10ED799F-7461-499B-969A-42F76A8BB5F9}">
+          <x14:formula1>
+            <xm:f>Data!$H$22:$H$24</xm:f>
+          </x14:formula1>
+          <xm:sqref>D6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AD6B5D3C-A12C-4B53-BD3C-F86457104F21}">
+          <x14:formula1>
+            <xm:f>Data!$H$17:$H$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>F6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{500CDD4D-3502-430A-9D92-5E02A24D1234}">
+          <x14:formula1>
+            <xm:f>Data!$H$27:$H$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>H6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{67728F4C-1251-40A7-80E6-5B8815AADCA0}">
+          <x14:formula1>
+            <xm:f>Data!$H$31:$H$33</xm:f>
+          </x14:formula1>
+          <xm:sqref>J6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1F105229-7CC1-45FF-9CB4-2E935325D0CE}">
+          <x14:formula1>
+            <xm:f>Data!$H$36:$H$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>L6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{55B9997E-F12F-4710-AEFC-40BCF9C98D16}">
+          <x14:formula1>
+            <xm:f>Data!$H$41:$H$51</xm:f>
+          </x14:formula1>
+          <xm:sqref>O6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{30713C3A-DA4B-44FC-BCFA-C6C0F5DE1DDB}">
+          <x14:formula1>
+            <xm:f>Data!$H$54:$H$60</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2BAD9088-851D-47B0-B6D3-3DAACA2009D9}">
+          <x14:formula1>
+            <xm:f>Data!$H$63:$H$65</xm:f>
+          </x14:formula1>
+          <xm:sqref>S6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B5479004-EB9B-4DBA-8A4B-11CB2CCB1B15}">
+          <x14:formula1>
+            <xm:f>UnderlyingPolicies!$A$1:$A$30</xm:f>
+          </x14:formula1>
+          <xm:sqref>D7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5E44A791-FDB8-4B09-AA3D-B8E160DC0F57}">
+          <x14:formula1>
+            <xm:f>Data!$O$25:$O$27</xm:f>
+          </x14:formula1>
+          <xm:sqref>B8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DDFBDFD5-A27A-4870-AC9D-3B9DC3A44A7F}">
+          <x14:formula1>
+            <xm:f>Data!$O$31:$O$35</xm:f>
+          </x14:formula1>
+          <xm:sqref>G8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3E6CC1A-563C-42D0-9792-F9F3973383F5}">
+          <x14:formula1>
+            <xm:f>Data!$O$43:$O$47</xm:f>
+          </x14:formula1>
+          <xm:sqref>I8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A6767F06-D18A-4C17-91F1-A1B4759D4179}">
+          <x14:formula1>
+            <xm:f>Data!$O$50:$O$55</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q8 S8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B078701F-4850-42D9-98D8-0B5C9DC2E88B}">
+          <x14:formula1>
+            <xm:f>Data!$U$25:$U$35</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D71F7B-4ADB-4D56-90D4-F764BF2C369B}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3614,7 +6098,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -3631,7 +6115,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -3648,16 +6132,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -3672,12 +6156,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F39E60-B723-4571-BBBF-ECF3E7527663}">
   <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3835,11 +6319,11 @@
         <v>18</v>
       </c>
       <c r="E8">
-        <f>'[3]XS Rating Step A Inputs'!$A$20</f>
+        <f>'[5]XS Rating Step A Inputs'!$A$20</f>
         <v>1</v>
       </c>
       <c r="F8" t="str">
-        <f>'[3]XS Rating Step A Inputs'!$A$21</f>
+        <f>'[5]XS Rating Step A Inputs'!$A$21</f>
         <v>Low Risk</v>
       </c>
       <c r="G8" s="14" t="str">
@@ -3864,11 +6348,11 @@
         <v>18</v>
       </c>
       <c r="E9">
-        <f>'[3]XS Rating Step A Inputs'!$B$20</f>
+        <f>'[5]XS Rating Step A Inputs'!$B$20</f>
         <v>2</v>
       </c>
       <c r="F9" t="str">
-        <f>'[3]XS Rating Step A Inputs'!$B$21</f>
+        <f>'[5]XS Rating Step A Inputs'!$B$21</f>
         <v>Low/Medium Risk</v>
       </c>
       <c r="G9" s="14" t="str">
@@ -3893,11 +6377,11 @@
         <v>18</v>
       </c>
       <c r="E10">
-        <f>'[3]XS Rating Step A Inputs'!$C$20</f>
+        <f>'[5]XS Rating Step A Inputs'!$C$20</f>
         <v>3</v>
       </c>
       <c r="F10" t="str">
-        <f>'[3]XS Rating Step A Inputs'!$C$21</f>
+        <f>'[5]XS Rating Step A Inputs'!$C$21</f>
         <v>Medium Risk</v>
       </c>
       <c r="G10" s="14" t="str">
@@ -3922,11 +6406,11 @@
         <v>18</v>
       </c>
       <c r="E11">
-        <f>'[3]XS Rating Step A Inputs'!$D$20</f>
+        <f>'[5]XS Rating Step A Inputs'!$D$20</f>
         <v>4</v>
       </c>
       <c r="F11" t="str">
-        <f>'[3]XS Rating Step A Inputs'!$D$21</f>
+        <f>'[5]XS Rating Step A Inputs'!$D$21</f>
         <v>Medium/High Risk</v>
       </c>
       <c r="G11" s="14" t="str">
@@ -3951,11 +6435,11 @@
         <v>18</v>
       </c>
       <c r="E12">
-        <f>'[3]XS Rating Step A Inputs'!$E$20</f>
+        <f>'[5]XS Rating Step A Inputs'!$E$20</f>
         <v>5</v>
       </c>
       <c r="F12" t="str">
-        <f>'[3]XS Rating Step A Inputs'!$E$21</f>
+        <f>'[5]XS Rating Step A Inputs'!$E$21</f>
         <v>High Risk</v>
       </c>
       <c r="G12" s="14" t="str">
@@ -4037,7 +6521,7 @@
         <v>110</v>
       </c>
       <c r="H16" t="str">
-        <f>'[3]Step 1'!$B$39</f>
+        <f>'[5]Step 1'!$B$39</f>
         <v>Significant M&amp;A Activity /Level of M&amp;A Concern</v>
       </c>
       <c r="O16" s="32" t="s">
@@ -4058,11 +6542,11 @@
         <v>18</v>
       </c>
       <c r="F17" t="str">
-        <f>'[3]Step 1'!$C$39</f>
+        <f>'[5]Step 1'!$C$39</f>
         <v>Activity within 1 year / Very high concern</v>
       </c>
       <c r="G17" t="str">
-        <f>'[3]Step 1'!$D$39</f>
+        <f>'[5]Step 1'!$D$39</f>
         <v>1.30-1.50</v>
       </c>
       <c r="H17" s="17" t="str">
@@ -4087,11 +6571,11 @@
         <v>18</v>
       </c>
       <c r="F18" t="str">
-        <f>'[3]Step 1'!$C$40</f>
+        <f>'[5]Step 1'!$C$40</f>
         <v>Activity within 1-3 years / Material-high high concern</v>
       </c>
       <c r="G18" t="str">
-        <f>'[3]Step 1'!$D$40</f>
+        <f>'[5]Step 1'!$D$40</f>
         <v>1.20-1.30</v>
       </c>
       <c r="H18" s="17" t="str">
@@ -4116,11 +6600,11 @@
         <v>18</v>
       </c>
       <c r="F19" t="str">
-        <f>'[3]Step 1'!$C$41</f>
+        <f>'[5]Step 1'!$C$41</f>
         <v>No activity in last 3 years / Low or no concern</v>
       </c>
       <c r="G19" t="str">
-        <f>'[3]Step 1'!$D$41</f>
+        <f>'[5]Step 1'!$D$41</f>
         <v>0.80-1.20</v>
       </c>
       <c r="H19" s="17" t="str">
@@ -4168,7 +6652,7 @@
         <v>110</v>
       </c>
       <c r="H21" t="str">
-        <f>'[3]Step 1'!$B$35</f>
+        <f>'[5]Step 1'!$B$35</f>
         <v>Number of Years in Operation</v>
       </c>
     </row>
@@ -4183,11 +6667,11 @@
         <v>18</v>
       </c>
       <c r="F22" t="str">
-        <f>'[3]Step 1'!$C$35</f>
+        <f>'[5]Step 1'!$C$35</f>
         <v>&lt; 3 years</v>
       </c>
       <c r="G22" t="str">
-        <f>'[3]Step 1'!$D$35</f>
+        <f>'[5]Step 1'!$D$35</f>
         <v>1.05-1.25</v>
       </c>
       <c r="H22" s="16" t="str">
@@ -4206,11 +6690,11 @@
         <v>18</v>
       </c>
       <c r="F23" s="23" t="str">
-        <f>'[3]Step 1'!$C$36</f>
+        <f>'[5]Step 1'!$C$36</f>
         <v>=&lt;3 years and &lt;5 years</v>
       </c>
       <c r="G23" t="str">
-        <f>'[3]Step 1'!$D$36</f>
+        <f>'[5]Step 1'!$D$36</f>
         <v>1.00-1.05</v>
       </c>
       <c r="H23" s="16" t="str">
@@ -4229,11 +6713,11 @@
         <v>18</v>
       </c>
       <c r="F24" t="str">
-        <f>'[3]Step 1'!$C$37</f>
+        <f>'[5]Step 1'!$C$37</f>
         <v>&gt;5 years</v>
       </c>
       <c r="G24" t="str">
-        <f>'[3]Step 1'!$D$37</f>
+        <f>'[5]Step 1'!$D$37</f>
         <v>0.85-1.00</v>
       </c>
       <c r="H24" s="16" t="str">
@@ -4281,7 +6765,7 @@
         <v>110</v>
       </c>
       <c r="H26" t="str">
-        <f>'[3]Step 1'!$B$43</f>
+        <f>'[5]Step 1'!$B$43</f>
         <v>SEC Offering</v>
       </c>
       <c r="O26" s="36" t="s">
@@ -4302,11 +6786,11 @@
         <v>20</v>
       </c>
       <c r="F27" t="str">
-        <f>'[3]Step 1'!$C$43</f>
+        <f>'[5]Step 1'!$C$43</f>
         <v>Within 1 year</v>
       </c>
       <c r="G27" t="str">
-        <f>'[3]Step 1'!$D$43</f>
+        <f>'[5]Step 1'!$D$43</f>
         <v>1.00-1.55</v>
       </c>
       <c r="H27" s="18" t="str">
@@ -4331,11 +6815,11 @@
         <v>18</v>
       </c>
       <c r="F28" t="str">
-        <f>'[3]Step 1'!$C$44</f>
+        <f>'[5]Step 1'!$C$44</f>
         <v>None within last 12 months</v>
       </c>
       <c r="G28" t="str">
-        <f>'[3]Step 1'!$D$44</f>
+        <f>'[5]Step 1'!$D$44</f>
         <v>0.90-1.20</v>
       </c>
       <c r="H28" s="18" t="str">
@@ -4378,7 +6862,7 @@
         <v>110</v>
       </c>
       <c r="H30" t="str">
-        <f>'[3]Step 1'!$B$46</f>
+        <f>'[5]Step 1'!$B$46</f>
         <v>D&amp;O Litigation</v>
       </c>
       <c r="O30" s="38" t="s">
@@ -4399,11 +6883,11 @@
         <v>18</v>
       </c>
       <c r="F31" t="str">
-        <f>'[3]Step 1'!$C$46</f>
+        <f>'[5]Step 1'!$C$46</f>
         <v>Within 1 year</v>
       </c>
       <c r="G31" t="str">
-        <f>'[3]Step 1'!$D$46</f>
+        <f>'[5]Step 1'!$D$46</f>
         <v>1.20-1.50</v>
       </c>
       <c r="H31" s="19" t="str">
@@ -4428,11 +6912,11 @@
         <v>18</v>
       </c>
       <c r="F32" t="str">
-        <f>'[3]Step 1'!$C$47</f>
+        <f>'[5]Step 1'!$C$47</f>
         <v>Within 1-5 years</v>
       </c>
       <c r="G32" t="str">
-        <f>'[3]Step 1'!$D$47</f>
+        <f>'[5]Step 1'!$D$47</f>
         <v>1.00-1.50</v>
       </c>
       <c r="H32" s="19" t="str">
@@ -4457,11 +6941,11 @@
         <v>18</v>
       </c>
       <c r="F33" t="str">
-        <f>'[3]Step 1'!$C$48</f>
+        <f>'[5]Step 1'!$C$48</f>
         <v>Within 5-10 years</v>
       </c>
       <c r="G33" t="str">
-        <f>'[3]Step 1'!$D$48</f>
+        <f>'[5]Step 1'!$D$48</f>
         <v>0.80-1.10</v>
       </c>
       <c r="H33" s="19" t="str">
@@ -4509,7 +6993,7 @@
         <v>110</v>
       </c>
       <c r="H35" t="str">
-        <f>'[3]Step 1'!$B$50</f>
+        <f>'[5]Step 1'!$B$50</f>
         <v>Other Litigation</v>
       </c>
       <c r="O35" s="39" t="s">
@@ -4530,11 +7014,11 @@
         <v>18</v>
       </c>
       <c r="F36" t="str">
-        <f>'[3]Step 1'!$C$50</f>
+        <f>'[5]Step 1'!$C$50</f>
         <v>Potential Cost &gt;3% of assets</v>
       </c>
       <c r="G36" t="str">
-        <f>'[3]Step 1'!$D$50</f>
+        <f>'[5]Step 1'!$D$50</f>
         <v>1.20-1.30</v>
       </c>
       <c r="H36" s="20" t="str">
@@ -4553,11 +7037,11 @@
         <v>20</v>
       </c>
       <c r="F37" t="str">
-        <f>'[3]Step 1'!$C$51</f>
+        <f>'[5]Step 1'!$C$51</f>
         <v>Potential Cost 1-3% of assets</v>
       </c>
       <c r="G37" t="str">
-        <f>'[3]Step 1'!$D$51</f>
+        <f>'[5]Step 1'!$D$51</f>
         <v>1.10-1.20</v>
       </c>
       <c r="H37" s="20" t="str">
@@ -4576,11 +7060,11 @@
         <v>18</v>
       </c>
       <c r="F38" t="str">
-        <f>'[3]Step 1'!$C$52</f>
+        <f>'[5]Step 1'!$C$52</f>
         <v>Potential Cost &lt;1% of assets</v>
       </c>
       <c r="G38" t="str">
-        <f>'[3]Step 1'!$D$52</f>
+        <f>'[5]Step 1'!$D$52</f>
         <v>0.80-1.10</v>
       </c>
       <c r="H38" s="20" t="str">
@@ -4619,7 +7103,7 @@
         <v>110</v>
       </c>
       <c r="H40" t="str">
-        <f>'[3]Step 1'!$B$56</f>
+        <f>'[5]Step 1'!$B$56</f>
         <v>Coinsurance re SEC claims</v>
       </c>
       <c r="O40" s="40" t="s">
@@ -4637,11 +7121,11 @@
         <v>18</v>
       </c>
       <c r="F41" s="25">
-        <f>'[3]Step 1'!$C$56</f>
+        <f>'[5]Step 1'!$C$56</f>
         <v>0</v>
       </c>
       <c r="G41">
-        <f>'[3]Step 1'!$D$56</f>
+        <f>'[5]Step 1'!$D$56</f>
         <v>1</v>
       </c>
       <c r="H41" s="26" t="str">
@@ -4660,11 +7144,11 @@
         <v>18</v>
       </c>
       <c r="F42" s="25">
-        <f>'[3]Step 1'!$C$57</f>
+        <f>'[5]Step 1'!$C$57</f>
         <v>0.05</v>
       </c>
       <c r="G42" t="str">
-        <f>'[3]Step 1'!$D$57</f>
+        <f>'[5]Step 1'!$D$57</f>
         <v>0.95-0.97</v>
       </c>
       <c r="H42" s="26" t="str">
@@ -4686,11 +7170,11 @@
         <v>18</v>
       </c>
       <c r="F43" s="25">
-        <f>'[3]Step 1'!$C$58</f>
+        <f>'[5]Step 1'!$C$58</f>
         <v>0.1</v>
       </c>
       <c r="G43" t="str">
-        <f>'[3]Step 1'!$D$58</f>
+        <f>'[5]Step 1'!$D$58</f>
         <v>0.90-0.94</v>
       </c>
       <c r="H43" s="26" t="str">
@@ -4712,11 +7196,11 @@
         <v>18</v>
       </c>
       <c r="F44" s="25">
-        <f>'[3]Step 1'!$C$59</f>
+        <f>'[5]Step 1'!$C$59</f>
         <v>0.15</v>
       </c>
       <c r="G44" t="str">
-        <f>'[3]Step 1'!$D$59</f>
+        <f>'[5]Step 1'!$D$59</f>
         <v>0.87-0.91</v>
       </c>
       <c r="H44" s="26" t="str">
@@ -4738,11 +7222,11 @@
         <v>18</v>
       </c>
       <c r="F45" s="25">
-        <f>'[3]Step 1'!$C$60</f>
+        <f>'[5]Step 1'!$C$60</f>
         <v>0.2</v>
       </c>
       <c r="G45" t="str">
-        <f>'[3]Step 1'!$D$60</f>
+        <f>'[5]Step 1'!$D$60</f>
         <v>0.84-0.88</v>
       </c>
       <c r="H45" s="26" t="str">
@@ -4767,11 +7251,11 @@
         <v>111</v>
       </c>
       <c r="F46" s="25">
-        <f>'[3]Step 1'!$C$61</f>
+        <f>'[5]Step 1'!$C$61</f>
         <v>0.25</v>
       </c>
       <c r="G46" t="str">
-        <f>'[3]Step 1'!$D$61</f>
+        <f>'[5]Step 1'!$D$61</f>
         <v>0.81-0.85</v>
       </c>
       <c r="H46" s="26" t="str">
@@ -4797,11 +7281,11 @@
         <v>0%</v>
       </c>
       <c r="F47" s="25">
-        <f>'[3]Step 1'!$C$62</f>
+        <f>'[5]Step 1'!$C$62</f>
         <v>0.3</v>
       </c>
       <c r="G47" t="str">
-        <f>'[3]Step 1'!$D$62</f>
+        <f>'[5]Step 1'!$D$62</f>
         <v>0.78-0.82</v>
       </c>
       <c r="H47" s="26" t="str">
@@ -4827,11 +7311,11 @@
         <v>5%</v>
       </c>
       <c r="F48" s="25">
-        <f>'[3]Step 1'!$C$63</f>
+        <f>'[5]Step 1'!$C$63</f>
         <v>0.35</v>
       </c>
       <c r="G48" t="str">
-        <f>'[3]Step 1'!$D$63</f>
+        <f>'[5]Step 1'!$D$63</f>
         <v>0.75-0.79</v>
       </c>
       <c r="H48" s="26" t="str">
@@ -4854,11 +7338,11 @@
         <v>10%</v>
       </c>
       <c r="F49" s="25">
-        <f>'[3]Step 1'!$C$64</f>
+        <f>'[5]Step 1'!$C$64</f>
         <v>0.4</v>
       </c>
       <c r="G49" t="str">
-        <f>'[3]Step 1'!$D$64</f>
+        <f>'[5]Step 1'!$D$64</f>
         <v>0.72-0.76</v>
       </c>
       <c r="H49" s="26" t="str">
@@ -4881,11 +7365,11 @@
         <v>15%</v>
       </c>
       <c r="F50" s="25">
-        <f>'[3]Step 1'!$C$65</f>
+        <f>'[5]Step 1'!$C$65</f>
         <v>0.45</v>
       </c>
       <c r="G50" t="str">
-        <f>'[3]Step 1'!$D$65</f>
+        <f>'[5]Step 1'!$D$65</f>
         <v>0.70-0.74</v>
       </c>
       <c r="H50" s="26" t="str">
@@ -4911,11 +7395,11 @@
         <v>20%</v>
       </c>
       <c r="F51" s="25">
-        <f>'[3]Step 1'!$C$66</f>
+        <f>'[5]Step 1'!$C$66</f>
         <v>0.5</v>
       </c>
       <c r="G51" t="str">
-        <f>'[3]Step 1'!$D$66</f>
+        <f>'[5]Step 1'!$D$66</f>
         <v>0.68-0.72</v>
       </c>
       <c r="H51" s="26" t="str">
@@ -4956,7 +7440,7 @@
         <v>110</v>
       </c>
       <c r="H53" t="str">
-        <f>'[3]Step 1'!$B$69</f>
+        <f>'[5]Step 1'!$B$69</f>
         <v>Industry Risk/Level of Confidence in Industry</v>
       </c>
       <c r="O53" t="s">
@@ -4969,11 +7453,11 @@
         <v>35%</v>
       </c>
       <c r="F54" t="str">
-        <f>'[3]Step 1'!$C$69</f>
+        <f>'[5]Step 1'!$C$69</f>
         <v>Very Confident</v>
       </c>
       <c r="G54" t="str">
-        <f>'[3]Step 1'!$D$69</f>
+        <f>'[5]Step 1'!$D$69</f>
         <v>0.70-0.85</v>
       </c>
       <c r="H54" s="19" t="str">
@@ -4990,11 +7474,11 @@
         <v>40%</v>
       </c>
       <c r="F55" t="str">
-        <f>'[3]Step 1'!$C$70</f>
+        <f>'[5]Step 1'!$C$70</f>
         <v>Confident</v>
       </c>
       <c r="G55" t="str">
-        <f>'[3]Step 1'!$D$70</f>
+        <f>'[5]Step 1'!$D$70</f>
         <v>0.85-1.00</v>
       </c>
       <c r="H55" s="19" t="str">
@@ -5011,11 +7495,11 @@
         <v>45%</v>
       </c>
       <c r="F56" t="str">
-        <f>'[3]Step 1'!$C$71</f>
+        <f>'[5]Step 1'!$C$71</f>
         <v>Comfortable</v>
       </c>
       <c r="G56">
-        <f>'[3]Step 1'!$D$71</f>
+        <f>'[5]Step 1'!$D$71</f>
         <v>1</v>
       </c>
       <c r="H56" s="19" t="str">
@@ -5029,11 +7513,11 @@
         <v>50%</v>
       </c>
       <c r="F57" t="str">
-        <f>'[3]Step 1'!$C$72</f>
+        <f>'[5]Step 1'!$C$72</f>
         <v>Low Concern</v>
       </c>
       <c r="G57" t="str">
-        <f>'[3]Step 1'!$D$72</f>
+        <f>'[5]Step 1'!$D$72</f>
         <v>1.00-1.15</v>
       </c>
       <c r="H57" s="19" t="str">
@@ -5043,11 +7527,11 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F58" t="str">
-        <f>'[3]Step 1'!$C$73</f>
+        <f>'[5]Step 1'!$C$73</f>
         <v>Material Concern</v>
       </c>
       <c r="G58" t="str">
-        <f>'[3]Step 1'!$D$73</f>
+        <f>'[5]Step 1'!$D$73</f>
         <v>1.15-1.35</v>
       </c>
       <c r="H58" s="19" t="str">
@@ -5057,11 +7541,11 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F59" t="str">
-        <f>'[3]Step 1'!$C$74</f>
+        <f>'[5]Step 1'!$C$74</f>
         <v>High Concern</v>
       </c>
       <c r="G59" t="str">
-        <f>'[3]Step 1'!$D$74</f>
+        <f>'[5]Step 1'!$D$74</f>
         <v>1.35-1.75</v>
       </c>
       <c r="H59" s="19" t="str">
@@ -5071,11 +7555,11 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F60" t="str">
-        <f>'[3]Step 1'!$C$75</f>
+        <f>'[5]Step 1'!$C$75</f>
         <v>Very High to Severe Concern</v>
       </c>
       <c r="G60" t="str">
-        <f>'[3]Step 1'!$D$75</f>
+        <f>'[5]Step 1'!$D$75</f>
         <v>1.75-1.25</v>
       </c>
       <c r="H60" s="19" t="str">
@@ -5091,17 +7575,17 @@
         <v>110</v>
       </c>
       <c r="H62" t="str">
-        <f>'[3]Step 1'!$B$77</f>
+        <f>'[5]Step 1'!$B$77</f>
         <v>Discovery (Extended Reporting)</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F63" t="str">
-        <f>'[3]Step 1'!$C$77</f>
+        <f>'[5]Step 1'!$C$77</f>
         <v>1 year</v>
       </c>
       <c r="G63">
-        <f>'[3]Step 1'!$D$77</f>
+        <f>'[4]Step 1'!$D$77</f>
         <v>1</v>
       </c>
       <c r="H63" s="22" t="str">
@@ -5111,30 +7595,30 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F64" t="str">
-        <f>'[3]Step 1'!$C$78</f>
+        <f>'[5]Step 1'!$C$78</f>
         <v>2 years</v>
       </c>
       <c r="G64" t="str">
-        <f>'[3]Step 1'!$D$78</f>
-        <v>175%-200%</v>
+        <f>'[4]Step 1'!$D$78</f>
+        <v>1.75-2.00</v>
       </c>
       <c r="H64" s="22" t="str">
         <f>_xlfn.CONCAT(F64, " (", G64, ")")</f>
-        <v>2 years (175%-200%)</v>
+        <v>2 years (1.75-2.00)</v>
       </c>
     </row>
     <row r="65" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F65" t="str">
-        <f>'[3]Step 1'!$C$79</f>
+        <f>'[5]Step 1'!$C$79</f>
         <v>3 years</v>
       </c>
       <c r="G65" t="str">
-        <f>'[3]Step 1'!$D$79</f>
-        <v>225%-250%</v>
+        <f>'[4]Step 1'!$D$79</f>
+        <v>2.25-2.50</v>
       </c>
       <c r="H65" s="22" t="str">
         <f>_xlfn.CONCAT(F65, " (", G65, ")")</f>
-        <v>3 years (225%-250%)</v>
+        <v>3 years (2.25-2.50)</v>
       </c>
     </row>
   </sheetData>
@@ -5142,7 +7626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF205112-CE8F-474E-9359-3AB3D8E94A28}">
   <dimension ref="A1:N34"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Batch files to run Robot scripts on Mac
</commit_message>
<xml_diff>
--- a/Data/FalconTestData.xlsx
+++ b/Data/FalconTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niraj\PycharmProjects\RFTSeleniumTutorial\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D9B0ED-5683-4A84-B06E-65CB5C586309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5063BC98-7429-4AA2-AA83-86CC920362EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{D770CC2D-6A6F-458D-97EA-D55BC517FB0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D770CC2D-6A6F-458D-97EA-D55BC517FB0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="12" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1244,27 +1244,27 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="E7" t="str">
-            <v>Bally</v>
+            <v>Amazon</v>
           </cell>
         </row>
         <row r="8">
           <cell r="E8" t="str">
-            <v>BALY</v>
+            <v>AMZN</v>
           </cell>
         </row>
         <row r="9">
           <cell r="E9">
-            <v>2300</v>
+            <v>1499722</v>
           </cell>
         </row>
         <row r="10">
           <cell r="E10">
-            <v>1863</v>
+            <v>469820</v>
           </cell>
         </row>
         <row r="11">
           <cell r="E11">
-            <v>961</v>
+            <v>33360</v>
           </cell>
         </row>
         <row r="32">
@@ -1277,21 +1277,39 @@
             <v>1</v>
           </cell>
         </row>
+        <row r="35">
+          <cell r="E35"/>
+        </row>
         <row r="37">
           <cell r="E37">
             <v>1</v>
           </cell>
         </row>
+        <row r="39">
+          <cell r="E39"/>
+        </row>
+        <row r="41">
+          <cell r="E41"/>
+        </row>
+        <row r="43">
+          <cell r="E43"/>
+        </row>
         <row r="44">
           <cell r="E44">
             <v>1</v>
           </cell>
         </row>
+        <row r="46">
+          <cell r="E46"/>
+        </row>
         <row r="48">
           <cell r="E48">
             <v>1</v>
           </cell>
         </row>
+        <row r="50">
+          <cell r="E50"/>
+        </row>
         <row r="52">
           <cell r="E52">
             <v>1</v>
@@ -1299,7 +1317,7 @@
         </row>
         <row r="54">
           <cell r="E54">
-            <v>0.95</v>
+            <v>0.9</v>
           </cell>
         </row>
         <row r="56">
@@ -1307,6 +1325,21 @@
             <v>1</v>
           </cell>
         </row>
+        <row r="66">
+          <cell r="E66"/>
+        </row>
+        <row r="69">
+          <cell r="E69"/>
+        </row>
+        <row r="75">
+          <cell r="E75"/>
+        </row>
+        <row r="77">
+          <cell r="E77"/>
+        </row>
+        <row r="79">
+          <cell r="E79"/>
+        </row>
         <row r="81">
           <cell r="E81">
             <v>1</v>
@@ -1418,8 +1451,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="16">
           <cell r="B16" t="str">
@@ -1427,25 +1460,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1483,27 +1516,27 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="E7" t="str">
-            <v>Amazon</v>
+            <v>Bally</v>
           </cell>
         </row>
         <row r="8">
           <cell r="E8" t="str">
-            <v>AMZN</v>
+            <v>BALY</v>
           </cell>
         </row>
         <row r="9">
           <cell r="E9">
-            <v>1499722</v>
+            <v>2300</v>
           </cell>
         </row>
         <row r="10">
           <cell r="E10">
-            <v>469820</v>
+            <v>1863</v>
           </cell>
         </row>
         <row r="11">
           <cell r="E11">
-            <v>33360</v>
+            <v>961</v>
           </cell>
         </row>
         <row r="32">
@@ -1516,21 +1549,39 @@
             <v>1</v>
           </cell>
         </row>
+        <row r="35">
+          <cell r="E35"/>
+        </row>
         <row r="37">
           <cell r="E37">
             <v>1</v>
           </cell>
         </row>
+        <row r="39">
+          <cell r="E39"/>
+        </row>
+        <row r="41">
+          <cell r="E41"/>
+        </row>
+        <row r="43">
+          <cell r="E43"/>
+        </row>
         <row r="44">
           <cell r="E44">
             <v>1</v>
           </cell>
         </row>
+        <row r="46">
+          <cell r="E46"/>
+        </row>
         <row r="48">
           <cell r="E48">
             <v>1</v>
           </cell>
         </row>
+        <row r="50">
+          <cell r="E50"/>
+        </row>
         <row r="52">
           <cell r="E52">
             <v>1</v>
@@ -1538,13 +1589,28 @@
         </row>
         <row r="54">
           <cell r="E54">
-            <v>0.9</v>
+            <v>0.95</v>
           </cell>
         </row>
         <row r="56">
           <cell r="E56">
             <v>1</v>
           </cell>
+        </row>
+        <row r="66">
+          <cell r="E66"/>
+        </row>
+        <row r="69">
+          <cell r="E69"/>
+        </row>
+        <row r="75">
+          <cell r="E75"/>
+        </row>
+        <row r="77">
+          <cell r="E77"/>
+        </row>
+        <row r="79">
+          <cell r="E79"/>
         </row>
         <row r="81">
           <cell r="E81">
@@ -1722,27 +1788,27 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="E7" t="str">
-            <v>Ulta Beauty</v>
+            <v>Intel</v>
           </cell>
         </row>
         <row r="8">
           <cell r="E8" t="str">
-            <v>ULTA</v>
+            <v>INTC</v>
           </cell>
         </row>
         <row r="9">
           <cell r="E9">
-            <v>19500</v>
+            <v>188510</v>
           </cell>
         </row>
         <row r="10">
           <cell r="E10">
-            <v>5100</v>
+            <v>168430</v>
           </cell>
         </row>
         <row r="11">
           <cell r="E11">
-            <v>8100</v>
+            <v>79020</v>
           </cell>
         </row>
         <row r="32">
@@ -1755,14 +1821,24 @@
             <v>1</v>
           </cell>
         </row>
-        <row r="44">
-          <cell r="E44">
+        <row r="37">
+          <cell r="E37">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="E41">
             <v>1</v>
           </cell>
         </row>
-        <row r="48">
-          <cell r="E48">
-            <v>0.8</v>
+        <row r="43">
+          <cell r="E43">
+            <v>1.02</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="E52">
+            <v>0.95</v>
           </cell>
         </row>
         <row r="54">
@@ -1770,14 +1846,24 @@
             <v>1</v>
           </cell>
         </row>
-        <row r="56">
-          <cell r="E56">
+        <row r="77">
+          <cell r="D77">
             <v>1</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="D78" t="str">
+            <v>1.75-2.00</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="D79" t="str">
+            <v>2.25-2.50</v>
           </cell>
         </row>
         <row r="81">
           <cell r="E81">
-            <v>0.8</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="82">
@@ -1797,7 +1883,7 @@
         </row>
         <row r="85">
           <cell r="E85">
-            <v>1.45</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="86">
@@ -1807,7 +1893,7 @@
         </row>
         <row r="87">
           <cell r="E87">
-            <v>1.26</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="88">
@@ -1837,7 +1923,7 @@
         </row>
         <row r="93">
           <cell r="E93">
-            <v>1</v>
+            <v>0.95</v>
           </cell>
         </row>
         <row r="94">
@@ -1857,12 +1943,12 @@
         </row>
         <row r="97">
           <cell r="E97">
-            <v>1</v>
+            <v>0.8</v>
           </cell>
         </row>
         <row r="98">
           <cell r="E98">
-            <v>1</v>
+            <v>0.8</v>
           </cell>
         </row>
         <row r="99">
@@ -1872,7 +1958,7 @@
         </row>
         <row r="100">
           <cell r="E100">
-            <v>1</v>
+            <v>1.5</v>
           </cell>
         </row>
         <row r="101">
@@ -1891,7 +1977,7 @@
       <sheetData sheetId="3">
         <row r="16">
           <cell r="B16" t="str">
-            <v>Public Organizations</v>
+            <v>Private Organizations</v>
           </cell>
         </row>
       </sheetData>
@@ -1920,6 +2006,222 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Legend"/>
+      <sheetName val="Step 1"/>
+      <sheetName val="Step 2"/>
+      <sheetName val="Step 3"/>
+      <sheetName val="XS Rating Algorithm"/>
+      <sheetName val="XS Final Premium Calculation"/>
+      <sheetName val="XS Rate Tables Sections A-F"/>
+      <sheetName val="XS RateTables SectionA-Georgia"/>
+      <sheetName val="XS Rate Tables Section G"/>
+      <sheetName val="XS Rate Tables State Exceptions"/>
+      <sheetName val="XS Rating Step A Inputs"/>
+      <sheetName val="XS Rating Step B-F Inputs"/>
+      <sheetName val="XS Rating Step G Inputs"/>
+      <sheetName val="Rating Plan Support --&gt;"/>
+      <sheetName val="Page 1"/>
+      <sheetName val="Page 2"/>
+      <sheetName val="Page 4"/>
+      <sheetName val="Page 5"/>
+      <sheetName val="Step 2a"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="7">
+          <cell r="E7" t="str">
+            <v>Microsoft</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="E8" t="str">
+            <v>MSFT</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>109000</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="E10">
+            <v>125000</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>600000</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="E32">
+            <v>0.65</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="E33">
+            <v>0.55000000000000004</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="E35"/>
+        </row>
+        <row r="37">
+          <cell r="E37">
+            <v>1.05</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="E39"/>
+        </row>
+        <row r="41">
+          <cell r="E41"/>
+        </row>
+        <row r="43">
+          <cell r="E43"/>
+        </row>
+        <row r="44">
+          <cell r="E44">
+            <v>1.1000000000000001</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="E46">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="E48"/>
+        </row>
+        <row r="50">
+          <cell r="E50"/>
+        </row>
+        <row r="52">
+          <cell r="E52"/>
+        </row>
+        <row r="54">
+          <cell r="E54">
+            <v>0.95</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="E56"/>
+        </row>
+        <row r="66">
+          <cell r="E66"/>
+        </row>
+        <row r="69">
+          <cell r="E69"/>
+        </row>
+        <row r="75">
+          <cell r="E75"/>
+        </row>
+        <row r="77">
+          <cell r="E77"/>
+        </row>
+        <row r="79">
+          <cell r="E79"/>
+        </row>
+        <row r="81">
+          <cell r="E81"/>
+        </row>
+        <row r="82">
+          <cell r="E82"/>
+        </row>
+        <row r="83">
+          <cell r="E83"/>
+        </row>
+        <row r="84">
+          <cell r="E84"/>
+        </row>
+        <row r="85">
+          <cell r="E85"/>
+        </row>
+        <row r="86">
+          <cell r="E86"/>
+        </row>
+        <row r="87">
+          <cell r="E87"/>
+        </row>
+        <row r="88">
+          <cell r="E88"/>
+        </row>
+        <row r="89">
+          <cell r="E89"/>
+        </row>
+        <row r="90">
+          <cell r="E90"/>
+        </row>
+        <row r="91">
+          <cell r="E91"/>
+        </row>
+        <row r="92">
+          <cell r="E92"/>
+        </row>
+        <row r="93">
+          <cell r="E93"/>
+        </row>
+        <row r="94">
+          <cell r="E94"/>
+        </row>
+        <row r="95">
+          <cell r="E95"/>
+        </row>
+        <row r="96">
+          <cell r="E96"/>
+        </row>
+        <row r="97">
+          <cell r="E97"/>
+        </row>
+        <row r="98">
+          <cell r="E98"/>
+        </row>
+        <row r="99">
+          <cell r="E99"/>
+        </row>
+        <row r="100">
+          <cell r="E100"/>
+        </row>
+        <row r="101">
+          <cell r="E101"/>
+        </row>
+        <row r="102">
+          <cell r="E102"/>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10">
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>Public Organizations</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1951,27 +2253,27 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="E7" t="str">
-            <v>Intel</v>
+            <v>Ulta Beauty</v>
           </cell>
         </row>
         <row r="8">
           <cell r="E8" t="str">
-            <v>INTC</v>
+            <v>ULTA</v>
           </cell>
         </row>
         <row r="9">
           <cell r="E9">
-            <v>188510</v>
+            <v>19500</v>
           </cell>
         </row>
         <row r="10">
           <cell r="E10">
-            <v>168430</v>
+            <v>5100</v>
           </cell>
         </row>
         <row r="11">
           <cell r="E11">
-            <v>79020</v>
+            <v>8100</v>
           </cell>
         </row>
         <row r="32">
@@ -1984,49 +2286,68 @@
             <v>1</v>
           </cell>
         </row>
+        <row r="35">
+          <cell r="E35"/>
+        </row>
         <row r="37">
-          <cell r="E37">
-            <v>0.9</v>
-          </cell>
+          <cell r="E37"/>
+        </row>
+        <row r="39">
+          <cell r="E39"/>
         </row>
         <row r="41">
-          <cell r="E41">
+          <cell r="E41"/>
+        </row>
+        <row r="43">
+          <cell r="E43"/>
+        </row>
+        <row r="44">
+          <cell r="E44">
             <v>1</v>
           </cell>
         </row>
-        <row r="43">
-          <cell r="E43">
-            <v>1.02</v>
-          </cell>
+        <row r="46">
+          <cell r="E46"/>
+        </row>
+        <row r="48">
+          <cell r="E48">
+            <v>0.8</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="E50"/>
         </row>
         <row r="52">
-          <cell r="E52">
-            <v>0.95</v>
-          </cell>
+          <cell r="E52"/>
         </row>
         <row r="54">
           <cell r="E54">
             <v>1</v>
           </cell>
         </row>
+        <row r="56">
+          <cell r="E56">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="E66"/>
+        </row>
+        <row r="69">
+          <cell r="E69"/>
+        </row>
+        <row r="75">
+          <cell r="E75"/>
+        </row>
         <row r="77">
-          <cell r="D77">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="D78" t="str">
-            <v>1.75-2.00</v>
-          </cell>
+          <cell r="E77"/>
         </row>
         <row r="79">
-          <cell r="D79" t="str">
-            <v>2.25-2.50</v>
-          </cell>
+          <cell r="E79"/>
         </row>
         <row r="81">
           <cell r="E81">
-            <v>1</v>
+            <v>0.8</v>
           </cell>
         </row>
         <row r="82">
@@ -2046,7 +2367,7 @@
         </row>
         <row r="85">
           <cell r="E85">
-            <v>1</v>
+            <v>1.45</v>
           </cell>
         </row>
         <row r="86">
@@ -2056,7 +2377,7 @@
         </row>
         <row r="87">
           <cell r="E87">
-            <v>1</v>
+            <v>1.26</v>
           </cell>
         </row>
         <row r="88">
@@ -2086,7 +2407,7 @@
         </row>
         <row r="93">
           <cell r="E93">
-            <v>0.95</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="94">
@@ -2106,12 +2427,12 @@
         </row>
         <row r="97">
           <cell r="E97">
-            <v>0.8</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="98">
           <cell r="E98">
-            <v>0.8</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="99">
@@ -2121,7 +2442,7 @@
         </row>
         <row r="100">
           <cell r="E100">
-            <v>1.5</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="101">
@@ -2135,406 +2456,22 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="16">
           <cell r="B16" t="str">
-            <v>Private Organizations</v>
+            <v>Public Organizations</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Legend"/>
-      <sheetName val="Step 1"/>
-      <sheetName val="Step 2"/>
-      <sheetName val="Step 3"/>
-      <sheetName val="XS Rating Algorithm"/>
-      <sheetName val="XS Final Premium Calculation"/>
-      <sheetName val="XS Rate Tables Sections A-F"/>
-      <sheetName val="XS RateTables SectionA-Georgia"/>
-      <sheetName val="XS Rate Tables Section G"/>
-      <sheetName val="XS Rate Tables State Exceptions"/>
-      <sheetName val="XS Rating Step A Inputs"/>
-      <sheetName val="XS Rating Step B-F Inputs"/>
-      <sheetName val="XS Rating Step G Inputs"/>
-      <sheetName val="Rating Plan Support --&gt;"/>
-      <sheetName val="Page 1"/>
-      <sheetName val="Page 2"/>
-      <sheetName val="Page 4"/>
-      <sheetName val="Page 5"/>
-      <sheetName val="Step 2a"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="35">
-          <cell r="B35" t="str">
-            <v>Number of Years in Operation</v>
-          </cell>
-          <cell r="C35" t="str">
-            <v>&lt; 3 years</v>
-          </cell>
-          <cell r="D35" t="str">
-            <v>1.05-1.25</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36" t="str">
-            <v>=&lt;3 years and &lt;5 years</v>
-          </cell>
-          <cell r="D36" t="str">
-            <v>1.00-1.05</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37" t="str">
-            <v>&gt;5 years</v>
-          </cell>
-          <cell r="D37" t="str">
-            <v>0.85-1.00</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39" t="str">
-            <v>Significant M&amp;A Activity /Level of M&amp;A Concern</v>
-          </cell>
-          <cell r="C39" t="str">
-            <v>Activity within 1 year / Very high concern</v>
-          </cell>
-          <cell r="D39" t="str">
-            <v>1.30-1.50</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40" t="str">
-            <v>Activity within 1-3 years / Material-high high concern</v>
-          </cell>
-          <cell r="D40" t="str">
-            <v>1.20-1.30</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41" t="str">
-            <v>No activity in last 3 years / Low or no concern</v>
-          </cell>
-          <cell r="D41" t="str">
-            <v>0.80-1.20</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43" t="str">
-            <v>SEC Offering</v>
-          </cell>
-          <cell r="C43" t="str">
-            <v>Within 1 year</v>
-          </cell>
-          <cell r="D43" t="str">
-            <v>1.00-1.55</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="C44" t="str">
-            <v>None within last 12 months</v>
-          </cell>
-          <cell r="D44" t="str">
-            <v>0.90-1.20</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46" t="str">
-            <v>D&amp;O Litigation</v>
-          </cell>
-          <cell r="C46" t="str">
-            <v>Within 1 year</v>
-          </cell>
-          <cell r="D46" t="str">
-            <v>1.20-1.50</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="C47" t="str">
-            <v>Within 1-5 years</v>
-          </cell>
-          <cell r="D47" t="str">
-            <v>1.00-1.50</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48" t="str">
-            <v>Within 5-10 years</v>
-          </cell>
-          <cell r="D48" t="str">
-            <v>0.80-1.10</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50" t="str">
-            <v>Other Litigation</v>
-          </cell>
-          <cell r="C50" t="str">
-            <v>Potential Cost &gt;3% of assets</v>
-          </cell>
-          <cell r="D50" t="str">
-            <v>1.20-1.30</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="C51" t="str">
-            <v>Potential Cost 1-3% of assets</v>
-          </cell>
-          <cell r="D51" t="str">
-            <v>1.10-1.20</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="C52" t="str">
-            <v>Potential Cost &lt;1% of assets</v>
-          </cell>
-          <cell r="D52" t="str">
-            <v>0.80-1.10</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56" t="str">
-            <v>Coinsurance re SEC claims</v>
-          </cell>
-          <cell r="C56">
-            <v>0</v>
-          </cell>
-          <cell r="D56">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="C57">
-            <v>0.05</v>
-          </cell>
-          <cell r="D57" t="str">
-            <v>0.95-0.97</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58">
-            <v>0.1</v>
-          </cell>
-          <cell r="D58" t="str">
-            <v>0.90-0.94</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59">
-            <v>0.15</v>
-          </cell>
-          <cell r="D59" t="str">
-            <v>0.87-0.91</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="C60">
-            <v>0.2</v>
-          </cell>
-          <cell r="D60" t="str">
-            <v>0.84-0.88</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="C61">
-            <v>0.25</v>
-          </cell>
-          <cell r="D61" t="str">
-            <v>0.81-0.85</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="C62">
-            <v>0.3</v>
-          </cell>
-          <cell r="D62" t="str">
-            <v>0.78-0.82</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="C63">
-            <v>0.35</v>
-          </cell>
-          <cell r="D63" t="str">
-            <v>0.75-0.79</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="C64">
-            <v>0.4</v>
-          </cell>
-          <cell r="D64" t="str">
-            <v>0.72-0.76</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="C65">
-            <v>0.45</v>
-          </cell>
-          <cell r="D65" t="str">
-            <v>0.70-0.74</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="C66">
-            <v>0.5</v>
-          </cell>
-          <cell r="D66" t="str">
-            <v>0.68-0.72</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="B69" t="str">
-            <v>Industry Risk/Level of Confidence in Industry</v>
-          </cell>
-          <cell r="C69" t="str">
-            <v>Very Confident</v>
-          </cell>
-          <cell r="D69" t="str">
-            <v>0.70-0.85</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="C70" t="str">
-            <v>Confident</v>
-          </cell>
-          <cell r="D70" t="str">
-            <v>0.85-1.00</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="C71" t="str">
-            <v>Comfortable</v>
-          </cell>
-          <cell r="D71">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="C72" t="str">
-            <v>Low Concern</v>
-          </cell>
-          <cell r="D72" t="str">
-            <v>1.00-1.15</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="C73" t="str">
-            <v>Material Concern</v>
-          </cell>
-          <cell r="D73" t="str">
-            <v>1.15-1.35</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="C74" t="str">
-            <v>High Concern</v>
-          </cell>
-          <cell r="D74" t="str">
-            <v>1.35-1.75</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="C75" t="str">
-            <v>Very High to Severe Concern</v>
-          </cell>
-          <cell r="D75" t="str">
-            <v>1.75-1.25</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="B77" t="str">
-            <v>Discovery (Extended Reporting)</v>
-          </cell>
-          <cell r="C77" t="str">
-            <v>1 year</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="C78" t="str">
-            <v>2 years</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="C79" t="str">
-            <v>3 years</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
-      <sheetData sheetId="10">
-        <row r="20">
-          <cell r="A20">
-            <v>1</v>
-          </cell>
-          <cell r="B20">
-            <v>2</v>
-          </cell>
-          <cell r="C20">
-            <v>3</v>
-          </cell>
-          <cell r="D20">
-            <v>4</v>
-          </cell>
-          <cell r="E20">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>Low Risk</v>
-          </cell>
-          <cell r="B21" t="str">
-            <v>Low/Medium Risk</v>
-          </cell>
-          <cell r="C21" t="str">
-            <v>Medium Risk</v>
-          </cell>
-          <cell r="D21" t="str">
-            <v>Medium/High Risk</v>
-          </cell>
-          <cell r="E21" t="str">
-            <v>High Risk</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
@@ -2543,6 +2480,10 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2573,87 +2514,356 @@
       <sheetName val="Step 2a"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
-        <row r="7">
-          <cell r="E7" t="str">
-            <v>Microsoft</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8" t="str">
-            <v>MSFT</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9">
-            <v>109000</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>125000</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>600000</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>0.65</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>0.55000000000000004</v>
+        <row r="35">
+          <cell r="B35" t="str">
+            <v>Number of Years in Operation</v>
+          </cell>
+          <cell r="C35" t="str">
+            <v>&lt; 3 years</v>
+          </cell>
+          <cell r="D35" t="str">
+            <v>1.05-1.25</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36" t="str">
+            <v>=&lt;3 years and &lt;5 years</v>
+          </cell>
+          <cell r="D36" t="str">
+            <v>1.00-1.05</v>
           </cell>
         </row>
         <row r="37">
-          <cell r="E37">
-            <v>1.05</v>
+          <cell r="C37" t="str">
+            <v>&gt;5 years</v>
+          </cell>
+          <cell r="D37" t="str">
+            <v>0.85-1.00</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39" t="str">
+            <v>Significant M&amp;A Activity /Level of M&amp;A Concern</v>
+          </cell>
+          <cell r="C39" t="str">
+            <v>Activity within 1 year / Very high concern</v>
+          </cell>
+          <cell r="D39" t="str">
+            <v>1.30-1.50</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="C40" t="str">
+            <v>Activity within 1-3 years / Material-high high concern</v>
+          </cell>
+          <cell r="D40" t="str">
+            <v>1.20-1.30</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="C41" t="str">
+            <v>No activity in last 3 years / Low or no concern</v>
+          </cell>
+          <cell r="D41" t="str">
+            <v>0.80-1.20</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43" t="str">
+            <v>SEC Offering</v>
+          </cell>
+          <cell r="C43" t="str">
+            <v>Within 1 year</v>
+          </cell>
+          <cell r="D43" t="str">
+            <v>1.00-1.55</v>
           </cell>
         </row>
         <row r="44">
-          <cell r="E44">
-            <v>1.1000000000000001</v>
+          <cell r="C44" t="str">
+            <v>None within last 12 months</v>
+          </cell>
+          <cell r="D44" t="str">
+            <v>0.90-1.20</v>
           </cell>
         </row>
         <row r="46">
-          <cell r="E46">
-            <v>1.2</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>0.95</v>
+          <cell r="B46" t="str">
+            <v>D&amp;O Litigation</v>
+          </cell>
+          <cell r="C46" t="str">
+            <v>Within 1 year</v>
+          </cell>
+          <cell r="D46" t="str">
+            <v>1.20-1.50</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="C47" t="str">
+            <v>Within 1-5 years</v>
+          </cell>
+          <cell r="D47" t="str">
+            <v>1.00-1.50</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="C48" t="str">
+            <v>Within 5-10 years</v>
+          </cell>
+          <cell r="D48" t="str">
+            <v>0.80-1.10</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="B50" t="str">
+            <v>Other Litigation</v>
+          </cell>
+          <cell r="C50" t="str">
+            <v>Potential Cost &gt;3% of assets</v>
+          </cell>
+          <cell r="D50" t="str">
+            <v>1.20-1.30</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="C51" t="str">
+            <v>Potential Cost 1-3% of assets</v>
+          </cell>
+          <cell r="D51" t="str">
+            <v>1.10-1.20</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="C52" t="str">
+            <v>Potential Cost &lt;1% of assets</v>
+          </cell>
+          <cell r="D52" t="str">
+            <v>0.80-1.10</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="B56" t="str">
+            <v>Coinsurance re SEC claims</v>
+          </cell>
+          <cell r="C56">
+            <v>0</v>
+          </cell>
+          <cell r="D56">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="C57">
+            <v>0.05</v>
+          </cell>
+          <cell r="D57" t="str">
+            <v>0.95-0.97</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="C58">
+            <v>0.1</v>
+          </cell>
+          <cell r="D58" t="str">
+            <v>0.90-0.94</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="C59">
+            <v>0.15</v>
+          </cell>
+          <cell r="D59" t="str">
+            <v>0.87-0.91</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="C60">
+            <v>0.2</v>
+          </cell>
+          <cell r="D60" t="str">
+            <v>0.84-0.88</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="C61">
+            <v>0.25</v>
+          </cell>
+          <cell r="D61" t="str">
+            <v>0.81-0.85</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="C62">
+            <v>0.3</v>
+          </cell>
+          <cell r="D62" t="str">
+            <v>0.78-0.82</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="C63">
+            <v>0.35</v>
+          </cell>
+          <cell r="D63" t="str">
+            <v>0.75-0.79</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="C64">
+            <v>0.4</v>
+          </cell>
+          <cell r="D64" t="str">
+            <v>0.72-0.76</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="C65">
+            <v>0.45</v>
+          </cell>
+          <cell r="D65" t="str">
+            <v>0.70-0.74</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="C66">
+            <v>0.5</v>
+          </cell>
+          <cell r="D66" t="str">
+            <v>0.68-0.72</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="B69" t="str">
+            <v>Industry Risk/Level of Confidence in Industry</v>
+          </cell>
+          <cell r="C69" t="str">
+            <v>Very Confident</v>
+          </cell>
+          <cell r="D69" t="str">
+            <v>0.70-0.85</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="C70" t="str">
+            <v>Confident</v>
+          </cell>
+          <cell r="D70" t="str">
+            <v>0.85-1.00</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="C71" t="str">
+            <v>Comfortable</v>
+          </cell>
+          <cell r="D71">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="C72" t="str">
+            <v>Low Concern</v>
+          </cell>
+          <cell r="D72" t="str">
+            <v>1.00-1.15</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="C73" t="str">
+            <v>Material Concern</v>
+          </cell>
+          <cell r="D73" t="str">
+            <v>1.15-1.35</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="C74" t="str">
+            <v>High Concern</v>
+          </cell>
+          <cell r="D74" t="str">
+            <v>1.35-1.75</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="C75" t="str">
+            <v>Very High to Severe Concern</v>
+          </cell>
+          <cell r="D75" t="str">
+            <v>1.75-1.25</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="B77" t="str">
+            <v>Discovery (Extended Reporting)</v>
+          </cell>
+          <cell r="C77" t="str">
+            <v>1 year</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="C78" t="str">
+            <v>2 years</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="C79" t="str">
+            <v>3 years</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
       <sheetData sheetId="10">
-        <row r="16">
-          <cell r="B16" t="str">
-            <v>Public Organizations</v>
+        <row r="20">
+          <cell r="A20">
+            <v>1</v>
+          </cell>
+          <cell r="B20">
+            <v>2</v>
+          </cell>
+          <cell r="C20">
+            <v>3</v>
+          </cell>
+          <cell r="D20">
+            <v>4</v>
+          </cell>
+          <cell r="E20">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>Low Risk</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>Low/Medium Risk</v>
+          </cell>
+          <cell r="C21" t="str">
+            <v>Medium Risk</v>
+          </cell>
+          <cell r="D21" t="str">
+            <v>Medium/High Risk</v>
+          </cell>
+          <cell r="E21" t="str">
+            <v>High Risk</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3103,7 +3313,7 @@
         <v>224</v>
       </c>
       <c r="B2" t="str">
-        <f>'[2]Step 1'!$E$7</f>
+        <f>'[1]Step 1'!$E$7</f>
         <v>Amazon</v>
       </c>
       <c r="C2" t="s">
@@ -3162,11 +3372,11 @@
         <v>33360000000</v>
       </c>
       <c r="E5" s="13" t="str">
-        <f>'[2]Step 1'!$E$8</f>
+        <f>'[1]Step 1'!$E$8</f>
         <v>AMZN</v>
       </c>
       <c r="F5" s="13" t="str">
-        <f>'[2]XS Rating Step A Inputs'!$B$16</f>
+        <f>'[1]XS Rating Step A Inputs'!$B$16</f>
         <v>Public Organizations</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -3199,159 +3409,159 @@
         <v>101</v>
       </c>
       <c r="B6" s="15">
-        <f>'[2]Step 1'!$E$32</f>
+        <f>'[1]Step 1'!$E$32</f>
         <v>1</v>
       </c>
       <c r="C6" s="15">
-        <f>'[2]Step 1'!$E$33</f>
+        <f>'[1]Step 1'!$E$33</f>
         <v>1</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="15" cm="1">
-        <f t="array" ref="E6">INDEX('[2]Step 1'!$E$35:'[2]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$35:'[2]Step 1'!$E$37),0))</f>
-        <v>1</v>
+      <c r="E6" s="15" t="e" cm="1">
+        <f t="array" ref="E6">INDEX('[1]Step 1'!$E$35:'[1]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$35:'[1]Step 1'!$E$37),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="15" cm="1">
-        <f t="array" ref="G6">INDEX('[2]Step 1'!$E$39:'[2]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$39:'[2]Step 1'!$E$41),0))</f>
-        <v>0.95</v>
+      <c r="G6" s="15" t="e" cm="1">
+        <f t="array" ref="G6">INDEX('[1]Step 1'!$E$39:'[1]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$39:'[1]Step 1'!$E$41),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>244</v>
       </c>
       <c r="I6" s="15" cm="1">
-        <f t="array" ref="I6">INDEX('[2]Step 1'!$E$43:'[2]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$43:'[2]Step 1'!$E$44),0))</f>
+        <f t="array" ref="I6">INDEX('[1]Step 1'!$E$43:'[1]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$43:'[1]Step 1'!$E$44),0))</f>
         <v>1</v>
       </c>
       <c r="J6" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="15" cm="1">
-        <f t="array" ref="K6">INDEX('[2]Step 1'!$E$46:'[2]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$46:'[2]Step 1'!$E$48),0))</f>
-        <v>1</v>
+      <c r="K6" s="15" t="e" cm="1">
+        <f t="array" ref="K6">INDEX('[1]Step 1'!$E$46:'[1]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$46:'[1]Step 1'!$E$48),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="M6" s="15" cm="1">
-        <f t="array" ref="M6">INDEX('[2]Step 1'!$E$50:'[2]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$50:'[2]Step 1'!$E$52),0))</f>
-        <v>1</v>
+      <c r="M6" s="15" t="e" cm="1">
+        <f t="array" ref="M6">INDEX('[1]Step 1'!$E$50:'[1]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$50:'[1]Step 1'!$E$52),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="N6" s="15">
-        <f>'[2]Step 1'!$E$54</f>
+        <f>'[1]Step 1'!$E$54</f>
         <v>0.9</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="P6" s="15" cm="1">
-        <f t="array" ref="P6">INDEX('[2]Step 1'!$E$56:'[2]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$56:'[2]Step 1'!$E$66),0))</f>
-        <v>1</v>
+      <c r="P6" s="15" t="e" cm="1">
+        <f t="array" ref="P6">INDEX('[1]Step 1'!$E$56:'[1]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$56:'[1]Step 1'!$E$66),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="Q6" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="R6" s="15" cm="1">
-        <f t="array" ref="R6">INDEX('[2]Step 1'!$E$69:'[2]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$69:'[2]Step 1'!$E$75),0))</f>
-        <v>0.9</v>
+      <c r="R6" s="15" t="e" cm="1">
+        <f t="array" ref="R6">INDEX('[1]Step 1'!$E$69:'[1]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$69:'[1]Step 1'!$E$75),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="S6" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="T6" s="15" cm="1">
-        <f t="array" ref="T6">INDEX('[2]Step 1'!$E$77:'[2]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$77:'[2]Step 1'!$E$79),0))</f>
-        <v>2</v>
+      <c r="T6" s="15" t="e" cm="1">
+        <f t="array" ref="T6">INDEX('[1]Step 1'!$E$77:'[1]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$77:'[1]Step 1'!$E$79),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="U6" s="15">
-        <f>'[2]Step 1'!$E$81</f>
+        <f>'[1]Step 1'!$E$81</f>
         <v>1</v>
       </c>
       <c r="V6" s="15">
-        <f>'[2]Step 1'!$E$82</f>
+        <f>'[1]Step 1'!$E$82</f>
         <v>0.9</v>
       </c>
       <c r="W6" s="15">
-        <f>'[2]Step 1'!$E$83</f>
+        <f>'[1]Step 1'!$E$83</f>
         <v>1</v>
       </c>
       <c r="X6" s="15">
-        <f>'[2]Step 1'!$E$84</f>
+        <f>'[1]Step 1'!$E$84</f>
         <v>0.95</v>
       </c>
       <c r="Y6" s="15">
-        <f>'[2]Step 1'!$E$85</f>
+        <f>'[1]Step 1'!$E$85</f>
         <v>1</v>
       </c>
       <c r="Z6" s="15">
-        <f>'[2]Step 1'!$E$86</f>
+        <f>'[1]Step 1'!$E$86</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AA6" s="15">
-        <f>'[2]Step 1'!$E$87</f>
+        <f>'[1]Step 1'!$E$87</f>
         <v>1</v>
       </c>
       <c r="AB6" s="15">
-        <f>'[2]Step 1'!$E$88</f>
+        <f>'[1]Step 1'!$E$88</f>
         <v>1</v>
       </c>
       <c r="AC6" s="15">
-        <f>'[2]Step 1'!$E$89</f>
+        <f>'[1]Step 1'!$E$89</f>
         <v>1</v>
       </c>
       <c r="AD6" s="15">
-        <f>'[2]Step 1'!$E$90</f>
+        <f>'[1]Step 1'!$E$90</f>
         <v>0.95</v>
       </c>
       <c r="AE6" s="15">
-        <f>'[2]Step 1'!$E$91</f>
+        <f>'[1]Step 1'!$E$91</f>
         <v>0.95</v>
       </c>
       <c r="AF6" s="15">
-        <f>'[2]Step 1'!$E$92</f>
+        <f>'[1]Step 1'!$E$92</f>
         <v>0.9</v>
       </c>
       <c r="AG6" s="15">
-        <f>'[2]Step 1'!$E$93</f>
+        <f>'[1]Step 1'!$E$93</f>
         <v>0.95</v>
       </c>
       <c r="AH6" s="15">
-        <f>'[2]Step 1'!$E$94</f>
+        <f>'[1]Step 1'!$E$94</f>
         <v>1</v>
       </c>
       <c r="AI6" s="15">
-        <f>'[2]Step 1'!$E$95</f>
+        <f>'[1]Step 1'!$E$95</f>
         <v>1</v>
       </c>
       <c r="AJ6" s="15">
-        <f>'[2]Step 1'!$E$96</f>
+        <f>'[1]Step 1'!$E$96</f>
         <v>1</v>
       </c>
       <c r="AK6" s="15">
-        <f>'[2]Step 1'!$E$97</f>
+        <f>'[1]Step 1'!$E$97</f>
         <v>1</v>
       </c>
       <c r="AL6" s="15">
-        <f>'[2]Step 1'!$E$98</f>
+        <f>'[1]Step 1'!$E$98</f>
         <v>1</v>
       </c>
       <c r="AM6" s="15">
-        <f>'[2]Step 1'!$E$99</f>
+        <f>'[1]Step 1'!$E$99</f>
         <v>0.95</v>
       </c>
       <c r="AN6" s="15">
-        <f>'[2]Step 1'!$E$100</f>
+        <f>'[1]Step 1'!$E$100</f>
         <v>1</v>
       </c>
       <c r="AO6" s="15">
-        <f>'[2]Step 1'!$E$101</f>
+        <f>'[1]Step 1'!$E$101</f>
         <v>1</v>
       </c>
       <c r="AP6" s="15">
-        <f>'[2]Step 1'!$E$102</f>
+        <f>'[1]Step 1'!$E$102</f>
         <v>1</v>
       </c>
     </row>
@@ -3452,15 +3662,15 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <f>'[2]Step 1'!$E$9</f>
+        <f>'[1]Step 1'!$E$9</f>
         <v>1499722</v>
       </c>
       <c r="C18" s="11">
-        <f>'[2]Step 1'!$E$10</f>
+        <f>'[1]Step 1'!$E$10</f>
         <v>469820</v>
       </c>
       <c r="D18" s="11">
-        <f>'[2]Step 1'!$E$11</f>
+        <f>'[1]Step 1'!$E$11</f>
         <v>33360</v>
       </c>
     </row>
@@ -3728,7 +3938,7 @@
         <v>224</v>
       </c>
       <c r="B2" t="str">
-        <f>'[1]Step 1'!$E$7</f>
+        <f>'[2]Step 1'!$E$7</f>
         <v>Bally</v>
       </c>
       <c r="C2" t="s">
@@ -3787,11 +3997,11 @@
         <v>961000000</v>
       </c>
       <c r="E5" s="13" t="str">
-        <f>'[1]Step 1'!$E$8</f>
+        <f>'[2]Step 1'!$E$8</f>
         <v>BALY</v>
       </c>
       <c r="F5" s="13" t="str">
-        <f>'[1]XS Rating Step A Inputs'!$B$16</f>
+        <f>'[2]XS Rating Step A Inputs'!$B$16</f>
         <v>Public Organizations</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -3824,159 +4034,159 @@
         <v>101</v>
       </c>
       <c r="B6" s="15">
-        <f>'[1]Step 1'!$E$32</f>
+        <f>'[2]Step 1'!$E$32</f>
         <v>1</v>
       </c>
       <c r="C6" s="15">
-        <f>'[1]Step 1'!$E$33</f>
+        <f>'[2]Step 1'!$E$33</f>
         <v>1</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="15" cm="1">
-        <f t="array" ref="E6">INDEX('[1]Step 1'!$E$35:'[1]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$35:'[1]Step 1'!$E$37),0))</f>
-        <v>1</v>
+      <c r="E6" s="15" t="e" cm="1">
+        <f t="array" ref="E6">INDEX('[2]Step 1'!$E$35:'[2]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$35:'[2]Step 1'!$E$37),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="G6" s="15" cm="1">
-        <f t="array" ref="G6">INDEX('[1]Step 1'!$E$39:'[1]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$39:'[1]Step 1'!$E$41),0))</f>
-        <v>0.95</v>
+      <c r="G6" s="15" t="e" cm="1">
+        <f t="array" ref="G6">INDEX('[2]Step 1'!$E$39:'[2]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$39:'[2]Step 1'!$E$41),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>104</v>
       </c>
       <c r="I6" s="15" cm="1">
-        <f t="array" ref="I6">INDEX('[1]Step 1'!$E$43:'[1]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$43:'[1]Step 1'!$E$44),0))</f>
+        <f t="array" ref="I6">INDEX('[2]Step 1'!$E$43:'[2]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$43:'[2]Step 1'!$E$44),0))</f>
         <v>1</v>
       </c>
       <c r="J6" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="15" cm="1">
-        <f t="array" ref="K6">INDEX('[1]Step 1'!$E$46:'[1]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$46:'[1]Step 1'!$E$48),0))</f>
-        <v>1</v>
+      <c r="K6" s="15" t="e" cm="1">
+        <f t="array" ref="K6">INDEX('[2]Step 1'!$E$46:'[2]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$46:'[2]Step 1'!$E$48),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="M6" s="15" cm="1">
-        <f t="array" ref="M6">INDEX('[1]Step 1'!$E$50:'[1]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$50:'[1]Step 1'!$E$52),0))</f>
-        <v>1</v>
+      <c r="M6" s="15" t="e" cm="1">
+        <f t="array" ref="M6">INDEX('[2]Step 1'!$E$50:'[2]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$50:'[2]Step 1'!$E$52),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="N6" s="15">
-        <f>'[1]Step 1'!$E$54</f>
+        <f>'[2]Step 1'!$E$54</f>
         <v>0.95</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="P6" s="15" cm="1">
-        <f t="array" ref="P6">INDEX('[1]Step 1'!$E$56:'[1]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$56:'[1]Step 1'!$E$66),0))</f>
-        <v>1</v>
+      <c r="P6" s="15" t="e" cm="1">
+        <f t="array" ref="P6">INDEX('[2]Step 1'!$E$56:'[2]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$56:'[2]Step 1'!$E$66),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="Q6" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="R6" s="15" cm="1">
-        <f t="array" ref="R6">INDEX('[1]Step 1'!$E$69:'[1]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$69:'[1]Step 1'!$E$75),0))</f>
-        <v>0.9</v>
+      <c r="R6" s="15" t="e" cm="1">
+        <f t="array" ref="R6">INDEX('[2]Step 1'!$E$69:'[2]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$69:'[2]Step 1'!$E$75),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="S6" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="T6" s="15" cm="1">
-        <f t="array" ref="T6">INDEX('[1]Step 1'!$E$77:'[1]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[1]Step 1'!$E$77:'[1]Step 1'!$E$79),0))</f>
-        <v>2</v>
+      <c r="T6" s="15" t="e" cm="1">
+        <f t="array" ref="T6">INDEX('[2]Step 1'!$E$77:'[2]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[2]Step 1'!$E$77:'[2]Step 1'!$E$79),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="U6" s="15">
-        <f>'[1]Step 1'!$E$81</f>
+        <f>'[2]Step 1'!$E$81</f>
         <v>1</v>
       </c>
       <c r="V6" s="15">
-        <f>'[1]Step 1'!$E$82</f>
+        <f>'[2]Step 1'!$E$82</f>
         <v>0.9</v>
       </c>
       <c r="W6" s="15">
-        <f>'[1]Step 1'!$E$83</f>
+        <f>'[2]Step 1'!$E$83</f>
         <v>1</v>
       </c>
       <c r="X6" s="15">
-        <f>'[1]Step 1'!$E$84</f>
+        <f>'[2]Step 1'!$E$84</f>
         <v>0.95</v>
       </c>
       <c r="Y6" s="15">
-        <f>'[1]Step 1'!$E$85</f>
+        <f>'[2]Step 1'!$E$85</f>
         <v>1</v>
       </c>
       <c r="Z6" s="15">
-        <f>'[1]Step 1'!$E$86</f>
+        <f>'[2]Step 1'!$E$86</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AA6" s="15">
-        <f>'[1]Step 1'!$E$87</f>
+        <f>'[2]Step 1'!$E$87</f>
         <v>1</v>
       </c>
       <c r="AB6" s="15">
-        <f>'[1]Step 1'!$E$88</f>
+        <f>'[2]Step 1'!$E$88</f>
         <v>1</v>
       </c>
       <c r="AC6" s="15">
-        <f>'[1]Step 1'!$E$89</f>
+        <f>'[2]Step 1'!$E$89</f>
         <v>1</v>
       </c>
       <c r="AD6" s="15">
-        <f>'[1]Step 1'!$E$90</f>
+        <f>'[2]Step 1'!$E$90</f>
         <v>0.95</v>
       </c>
       <c r="AE6" s="15">
-        <f>'[1]Step 1'!$E$91</f>
+        <f>'[2]Step 1'!$E$91</f>
         <v>0.95</v>
       </c>
       <c r="AF6" s="15">
-        <f>'[1]Step 1'!$E$92</f>
+        <f>'[2]Step 1'!$E$92</f>
         <v>0.9</v>
       </c>
       <c r="AG6" s="15">
-        <f>'[1]Step 1'!$E$93</f>
+        <f>'[2]Step 1'!$E$93</f>
         <v>0.95</v>
       </c>
       <c r="AH6" s="15">
-        <f>'[1]Step 1'!$E$94</f>
+        <f>'[2]Step 1'!$E$94</f>
         <v>1</v>
       </c>
       <c r="AI6" s="15">
-        <f>'[1]Step 1'!$E$95</f>
+        <f>'[2]Step 1'!$E$95</f>
         <v>1</v>
       </c>
       <c r="AJ6" s="15">
-        <f>'[1]Step 1'!$E$96</f>
+        <f>'[2]Step 1'!$E$96</f>
         <v>1</v>
       </c>
       <c r="AK6" s="15">
-        <f>'[1]Step 1'!$E$97</f>
+        <f>'[2]Step 1'!$E$97</f>
         <v>1</v>
       </c>
       <c r="AL6" s="15">
-        <f>'[1]Step 1'!$E$98</f>
+        <f>'[2]Step 1'!$E$98</f>
         <v>1</v>
       </c>
       <c r="AM6" s="15">
-        <f>'[1]Step 1'!$E$99</f>
+        <f>'[2]Step 1'!$E$99</f>
         <v>0.95</v>
       </c>
       <c r="AN6" s="15">
-        <f>'[1]Step 1'!$E$100</f>
+        <f>'[2]Step 1'!$E$100</f>
         <v>1</v>
       </c>
       <c r="AO6" s="15">
-        <f>'[1]Step 1'!$E$101</f>
+        <f>'[2]Step 1'!$E$101</f>
         <v>1</v>
       </c>
       <c r="AP6" s="15">
-        <f>'[1]Step 1'!$E$102</f>
+        <f>'[2]Step 1'!$E$102</f>
         <v>1</v>
       </c>
     </row>
@@ -4077,15 +4287,15 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <f>'[1]Step 1'!$E$9</f>
+        <f>'[2]Step 1'!$E$9</f>
         <v>2300</v>
       </c>
       <c r="C18" s="11">
-        <f>'[1]Step 1'!$E$10</f>
+        <f>'[2]Step 1'!$E$10</f>
         <v>1863</v>
       </c>
       <c r="D18" s="11">
-        <f>'[1]Step 1'!$E$11</f>
+        <f>'[2]Step 1'!$E$11</f>
         <v>961</v>
       </c>
     </row>
@@ -4208,8 +4418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7431024C-B1CA-4198-BB91-2F4C2F294154}">
   <dimension ref="A1:AP18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4353,7 +4563,7 @@
         <v>224</v>
       </c>
       <c r="B2" t="str">
-        <f>'[4]Step 1'!$E$7</f>
+        <f>'[3]Step 1'!$E$7</f>
         <v>Intel</v>
       </c>
       <c r="C2" t="s">
@@ -4388,11 +4598,11 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="D4" t="str">
         <f>IFERROR(VLOOKUP(C4,Data!$A:$B,2,FALSE)," ")</f>
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
@@ -4412,11 +4622,11 @@
         <v>79020000000</v>
       </c>
       <c r="E5" s="13" t="str">
-        <f>'[4]Step 1'!$E$8</f>
+        <f>'[3]Step 1'!$E$8</f>
         <v>INTC</v>
       </c>
       <c r="F5" s="13" t="str">
-        <f>'[4]XS Rating Step A Inputs'!$B$16</f>
+        <f>'[3]XS Rating Step A Inputs'!$B$16</f>
         <v>Private Organizations</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -4449,159 +4659,159 @@
         <v>101</v>
       </c>
       <c r="B6" s="15">
-        <f>'[4]Step 1'!$E$32</f>
+        <f>'[3]Step 1'!$E$32</f>
         <v>1</v>
       </c>
       <c r="C6" s="15">
-        <f>'[4]Step 1'!$E$33</f>
+        <f>'[3]Step 1'!$E$33</f>
         <v>1</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>102</v>
       </c>
       <c r="E6" s="15" cm="1">
-        <f t="array" ref="E6">INDEX('[4]Step 1'!$E$35:'[4]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$35:'[4]Step 1'!$E$37),0))</f>
+        <f t="array" ref="E6">INDEX('[3]Step 1'!$E$35:'[3]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$35:'[3]Step 1'!$E$37),0))</f>
         <v>0.9</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>103</v>
       </c>
       <c r="G6" s="15" cm="1">
-        <f t="array" ref="G6">INDEX('[4]Step 1'!$E$39:'[4]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$39:'[4]Step 1'!$E$41),0))</f>
+        <f t="array" ref="G6">INDEX('[3]Step 1'!$E$39:'[3]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$39:'[3]Step 1'!$E$41),0))</f>
         <v>1</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>244</v>
       </c>
       <c r="I6" s="15" cm="1">
-        <f t="array" ref="I6">INDEX('[4]Step 1'!$E$43:'[4]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$43:'[4]Step 1'!$E$44),0))</f>
+        <f t="array" ref="I6">INDEX('[3]Step 1'!$E$43:'[3]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$43:'[3]Step 1'!$E$44),0))</f>
         <v>1.02</v>
       </c>
       <c r="J6" s="19" t="s">
         <v>245</v>
       </c>
       <c r="K6" s="15" cm="1">
-        <f t="array" ref="K6">INDEX('[4]Step 1'!$E$46:'[4]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$46:'[4]Step 1'!$E$48),0))</f>
+        <f t="array" ref="K6">INDEX('[3]Step 1'!$E$46:'[3]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$46:'[3]Step 1'!$E$48),0))</f>
         <v>1.36</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>106</v>
       </c>
       <c r="M6" s="15" cm="1">
-        <f t="array" ref="M6">INDEX('[4]Step 1'!$E$50:'[4]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$50:'[4]Step 1'!$E$52),0))</f>
+        <f t="array" ref="M6">INDEX('[3]Step 1'!$E$50:'[3]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$50:'[3]Step 1'!$E$52),0))</f>
         <v>0.95</v>
       </c>
       <c r="N6" s="15">
-        <f>'[4]Step 1'!$E$54</f>
+        <f>'[3]Step 1'!$E$54</f>
         <v>1</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>246</v>
       </c>
       <c r="P6" s="15" cm="1">
-        <f t="array" ref="P6">INDEX('[4]Step 1'!$E$56:'[4]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$56:'[4]Step 1'!$E$66),0))</f>
+        <f t="array" ref="P6">INDEX('[3]Step 1'!$E$56:'[3]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$56:'[3]Step 1'!$E$66),0))</f>
         <v>0.81</v>
       </c>
       <c r="Q6" s="19" t="s">
         <v>247</v>
       </c>
       <c r="R6" s="15" cm="1">
-        <f t="array" ref="R6">INDEX('[4]Step 1'!$E$69:'[4]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$69:'[4]Step 1'!$E$75),0))</f>
+        <f t="array" ref="R6">INDEX('[3]Step 1'!$E$69:'[3]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$69:'[3]Step 1'!$E$75),0))</f>
         <v>1.05</v>
       </c>
       <c r="S6" s="22" t="s">
         <v>109</v>
       </c>
       <c r="T6" s="15" cm="1">
-        <f t="array" ref="T6">INDEX('[4]Step 1'!$E$77:'[4]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$77:'[4]Step 1'!$E$79),0))</f>
+        <f t="array" ref="T6">INDEX('[3]Step 1'!$E$77:'[3]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$77:'[3]Step 1'!$E$79),0))</f>
         <v>2</v>
       </c>
       <c r="U6" s="15">
-        <f>'[4]Step 1'!$E$81</f>
+        <f>'[3]Step 1'!$E$81</f>
         <v>1</v>
       </c>
       <c r="V6" s="15">
-        <f>'[4]Step 1'!$E$82</f>
+        <f>'[3]Step 1'!$E$82</f>
         <v>0.9</v>
       </c>
       <c r="W6" s="15">
-        <f>'[4]Step 1'!$E$83</f>
+        <f>'[3]Step 1'!$E$83</f>
         <v>1</v>
       </c>
       <c r="X6" s="15">
-        <f>'[4]Step 1'!$E$84</f>
+        <f>'[3]Step 1'!$E$84</f>
         <v>0.95</v>
       </c>
       <c r="Y6" s="15">
-        <f>'[4]Step 1'!$E$85</f>
+        <f>'[3]Step 1'!$E$85</f>
         <v>1</v>
       </c>
       <c r="Z6" s="15">
-        <f>'[4]Step 1'!$E$86</f>
+        <f>'[3]Step 1'!$E$86</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AA6" s="15">
-        <f>'[4]Step 1'!$E$87</f>
+        <f>'[3]Step 1'!$E$87</f>
         <v>1</v>
       </c>
       <c r="AB6" s="15">
-        <f>'[4]Step 1'!$E$88</f>
+        <f>'[3]Step 1'!$E$88</f>
         <v>1</v>
       </c>
       <c r="AC6" s="15">
-        <f>'[4]Step 1'!$E$89</f>
+        <f>'[3]Step 1'!$E$89</f>
         <v>1</v>
       </c>
       <c r="AD6" s="15">
-        <f>'[4]Step 1'!$E$90</f>
+        <f>'[3]Step 1'!$E$90</f>
         <v>0.95</v>
       </c>
       <c r="AE6" s="15">
-        <f>'[4]Step 1'!$E$91</f>
+        <f>'[3]Step 1'!$E$91</f>
         <v>0.95</v>
       </c>
       <c r="AF6" s="15">
-        <f>'[4]Step 1'!$E$92</f>
+        <f>'[3]Step 1'!$E$92</f>
         <v>0.9</v>
       </c>
       <c r="AG6" s="15">
-        <f>'[4]Step 1'!$E$93</f>
+        <f>'[3]Step 1'!$E$93</f>
         <v>0.95</v>
       </c>
       <c r="AH6" s="15">
-        <f>'[4]Step 1'!$E$94</f>
+        <f>'[3]Step 1'!$E$94</f>
         <v>1</v>
       </c>
       <c r="AI6" s="15">
-        <f>'[4]Step 1'!$E$95</f>
+        <f>'[3]Step 1'!$E$95</f>
         <v>1</v>
       </c>
       <c r="AJ6" s="15">
-        <f>'[4]Step 1'!$E$96</f>
+        <f>'[3]Step 1'!$E$96</f>
         <v>1</v>
       </c>
       <c r="AK6" s="15">
-        <f>'[4]Step 1'!$E$97</f>
+        <f>'[3]Step 1'!$E$97</f>
         <v>0.8</v>
       </c>
       <c r="AL6" s="15">
-        <f>'[4]Step 1'!$E$98</f>
+        <f>'[3]Step 1'!$E$98</f>
         <v>0.8</v>
       </c>
       <c r="AM6" s="15">
-        <f>'[4]Step 1'!$E$99</f>
+        <f>'[3]Step 1'!$E$99</f>
         <v>0.95</v>
       </c>
       <c r="AN6" s="15">
-        <f>'[4]Step 1'!$E$100</f>
+        <f>'[3]Step 1'!$E$100</f>
         <v>1.5</v>
       </c>
       <c r="AO6" s="15">
-        <f>'[4]Step 1'!$E$101</f>
+        <f>'[3]Step 1'!$E$101</f>
         <v>1</v>
       </c>
       <c r="AP6" s="15">
-        <f>'[4]Step 1'!$E$102</f>
+        <f>'[3]Step 1'!$E$102</f>
         <v>1</v>
       </c>
     </row>
@@ -4610,10 +4820,10 @@
         <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -4637,7 +4847,7 @@
       </c>
       <c r="F8" t="str">
         <f>D4</f>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G8" t="s">
         <v>205</v>
@@ -4646,10 +4856,10 @@
         <v>45</v>
       </c>
       <c r="I8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J8">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="K8">
         <v>5</v>
@@ -4702,15 +4912,15 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <f>'[4]Step 1'!$E$9</f>
+        <f>'[3]Step 1'!$E$9</f>
         <v>188510</v>
       </c>
       <c r="C18" s="11">
-        <f>'[4]Step 1'!$E$10</f>
+        <f>'[3]Step 1'!$E$10</f>
         <v>168430</v>
       </c>
       <c r="D18" s="11">
-        <f>'[4]Step 1'!$E$11</f>
+        <f>'[3]Step 1'!$E$11</f>
         <v>79020</v>
       </c>
     </row>
@@ -4978,7 +5188,7 @@
         <v>224</v>
       </c>
       <c r="B2" t="str">
-        <f>'[6]Step 1'!$E$7</f>
+        <f>'[4]Step 1'!$E$7</f>
         <v>Microsoft</v>
       </c>
       <c r="C2" t="s">
@@ -5037,11 +5247,11 @@
         <v>600000000000</v>
       </c>
       <c r="E5" s="13" t="str">
-        <f>'[6]Step 1'!$E$8</f>
+        <f>'[4]Step 1'!$E$8</f>
         <v>MSFT</v>
       </c>
       <c r="F5" s="13" t="str">
-        <f>'[6]XS Rating Step A Inputs'!$B$16</f>
+        <f>'[4]XS Rating Step A Inputs'!$B$16</f>
         <v>Public Organizations</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -5074,159 +5284,159 @@
         <v>101</v>
       </c>
       <c r="B6" s="15">
-        <f>'[6]Step 1'!$E$32</f>
+        <f>'[4]Step 1'!$E$32</f>
         <v>0.65</v>
       </c>
       <c r="C6" s="15">
-        <f>'[6]Step 1'!$E$33</f>
+        <f>'[4]Step 1'!$E$33</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="E6" s="15" cm="1">
-        <f t="array" ref="E6">INDEX('[6]Step 1'!$E$35:'[6]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$35:'[6]Step 1'!$E$37),0))</f>
-        <v>1.05</v>
+      <c r="E6" s="15" t="e" cm="1">
+        <f t="array" ref="E6">INDEX('[4]Step 1'!$E$35:'[4]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$35:'[4]Step 1'!$E$37),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="G6" s="15" cm="1">
-        <f t="array" ref="G6">INDEX('[6]Step 1'!$E$39:'[6]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$39:'[6]Step 1'!$E$41),0))</f>
-        <v>1.25</v>
+      <c r="G6" s="15" t="e" cm="1">
+        <f t="array" ref="G6">INDEX('[4]Step 1'!$E$39:'[4]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$39:'[4]Step 1'!$E$41),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>104</v>
       </c>
       <c r="I6" s="15" cm="1">
-        <f t="array" ref="I6">INDEX('[6]Step 1'!$E$43:'[6]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$43:'[6]Step 1'!$E$44),0))</f>
+        <f t="array" ref="I6">INDEX('[4]Step 1'!$E$43:'[4]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$43:'[4]Step 1'!$E$44),0))</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="J6" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="K6" s="15" cm="1">
-        <f t="array" ref="K6">INDEX('[6]Step 1'!$E$46:'[6]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$46:'[6]Step 1'!$E$48),0))</f>
-        <v>1.2</v>
+      <c r="K6" s="15" t="e" cm="1">
+        <f t="array" ref="K6">INDEX('[4]Step 1'!$E$46:'[4]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$46:'[4]Step 1'!$E$48),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="M6" s="15" cm="1">
-        <f t="array" ref="M6">INDEX('[6]Step 1'!$E$50:'[6]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$50:'[6]Step 1'!$E$52),0))</f>
-        <v>1.1000000000000001</v>
+      <c r="M6" s="15" t="e" cm="1">
+        <f t="array" ref="M6">INDEX('[4]Step 1'!$E$50:'[4]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$50:'[4]Step 1'!$E$52),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="N6" s="15">
-        <f>'[6]Step 1'!$E$54</f>
+        <f>'[4]Step 1'!$E$54</f>
         <v>0.95</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="P6" s="15" cm="1">
-        <f t="array" ref="P6">INDEX('[6]Step 1'!$E$56:'[6]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$56:'[6]Step 1'!$E$66),0))</f>
-        <v>0.93</v>
+      <c r="P6" s="15" t="e" cm="1">
+        <f t="array" ref="P6">INDEX('[4]Step 1'!$E$56:'[4]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$56:'[4]Step 1'!$E$66),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="Q6" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="R6" s="15" cm="1">
-        <f t="array" ref="R6">INDEX('[6]Step 1'!$E$69:'[6]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$69:'[6]Step 1'!$E$75),0))</f>
-        <v>1</v>
+      <c r="R6" s="15" t="e" cm="1">
+        <f t="array" ref="R6">INDEX('[4]Step 1'!$E$69:'[4]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$69:'[4]Step 1'!$E$75),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="S6" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="T6" s="15" cm="1">
-        <f t="array" ref="T6">INDEX('[6]Step 1'!$E$77:'[6]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[6]Step 1'!$E$77:'[6]Step 1'!$E$79),0))</f>
-        <v>1.75</v>
+      <c r="T6" s="15" t="e" cm="1">
+        <f t="array" ref="T6">INDEX('[4]Step 1'!$E$77:'[4]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[4]Step 1'!$E$77:'[4]Step 1'!$E$79),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="U6" s="15">
-        <f>'[6]Step 1'!$E$81</f>
+        <f>'[4]Step 1'!$E$81</f>
         <v>0</v>
       </c>
       <c r="V6" s="15">
-        <f>'[6]Step 1'!$E$82</f>
+        <f>'[4]Step 1'!$E$82</f>
         <v>0</v>
       </c>
       <c r="W6" s="15">
-        <f>'[6]Step 1'!$E$83</f>
+        <f>'[4]Step 1'!$E$83</f>
         <v>0</v>
       </c>
       <c r="X6" s="15">
-        <f>'[6]Step 1'!$E$84</f>
+        <f>'[4]Step 1'!$E$84</f>
         <v>0</v>
       </c>
       <c r="Y6" s="15">
-        <f>'[6]Step 1'!$E$85</f>
+        <f>'[4]Step 1'!$E$85</f>
         <v>0</v>
       </c>
       <c r="Z6" s="15">
-        <f>'[6]Step 1'!$E$86</f>
+        <f>'[4]Step 1'!$E$86</f>
         <v>0</v>
       </c>
       <c r="AA6" s="15">
-        <f>'[6]Step 1'!$E$87</f>
+        <f>'[4]Step 1'!$E$87</f>
         <v>0</v>
       </c>
       <c r="AB6" s="15">
-        <f>'[6]Step 1'!$E$88</f>
+        <f>'[4]Step 1'!$E$88</f>
         <v>0</v>
       </c>
       <c r="AC6" s="15">
-        <f>'[6]Step 1'!$E$89</f>
+        <f>'[4]Step 1'!$E$89</f>
         <v>0</v>
       </c>
       <c r="AD6" s="15">
-        <f>'[6]Step 1'!$E$90</f>
+        <f>'[4]Step 1'!$E$90</f>
         <v>0</v>
       </c>
       <c r="AE6" s="15">
-        <f>'[6]Step 1'!$E$91</f>
+        <f>'[4]Step 1'!$E$91</f>
         <v>0</v>
       </c>
       <c r="AF6" s="15">
-        <f>'[6]Step 1'!$E$92</f>
+        <f>'[4]Step 1'!$E$92</f>
         <v>0</v>
       </c>
       <c r="AG6" s="15">
-        <f>'[6]Step 1'!$E$93</f>
+        <f>'[4]Step 1'!$E$93</f>
         <v>0</v>
       </c>
       <c r="AH6" s="15">
-        <f>'[6]Step 1'!$E$94</f>
+        <f>'[4]Step 1'!$E$94</f>
         <v>0</v>
       </c>
       <c r="AI6" s="15">
-        <f>'[6]Step 1'!$E$95</f>
+        <f>'[4]Step 1'!$E$95</f>
         <v>0</v>
       </c>
       <c r="AJ6" s="15">
-        <f>'[6]Step 1'!$E$96</f>
+        <f>'[4]Step 1'!$E$96</f>
         <v>0</v>
       </c>
       <c r="AK6" s="15">
-        <f>'[6]Step 1'!$E$97</f>
+        <f>'[4]Step 1'!$E$97</f>
         <v>0</v>
       </c>
       <c r="AL6" s="15">
-        <f>'[6]Step 1'!$E$98</f>
+        <f>'[4]Step 1'!$E$98</f>
         <v>0</v>
       </c>
       <c r="AM6" s="15">
-        <f>'[6]Step 1'!$E$99</f>
+        <f>'[4]Step 1'!$E$99</f>
         <v>0</v>
       </c>
       <c r="AN6" s="15">
-        <f>'[6]Step 1'!$E$100</f>
+        <f>'[4]Step 1'!$E$100</f>
         <v>0</v>
       </c>
       <c r="AO6" s="15">
-        <f>'[6]Step 1'!$E$101</f>
+        <f>'[4]Step 1'!$E$101</f>
         <v>0</v>
       </c>
       <c r="AP6" s="15">
-        <f>'[6]Step 1'!$E$102</f>
+        <f>'[4]Step 1'!$E$102</f>
         <v>0</v>
       </c>
     </row>
@@ -5327,15 +5537,15 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <f>'[6]Step 1'!$E$9</f>
+        <f>'[4]Step 1'!$E$9</f>
         <v>109000</v>
       </c>
       <c r="C18" s="11">
-        <f>'[6]Step 1'!$E$10</f>
+        <f>'[4]Step 1'!$E$10</f>
         <v>125000</v>
       </c>
       <c r="D18" s="11">
-        <f>'[6]Step 1'!$E$11</f>
+        <f>'[4]Step 1'!$E$11</f>
         <v>600000</v>
       </c>
     </row>
@@ -5458,7 +5668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515B94FA-5A74-4B2F-AE46-2F448621C2E3}">
   <dimension ref="A1:AP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
@@ -5603,7 +5813,7 @@
         <v>224</v>
       </c>
       <c r="B2" t="str">
-        <f>'[3]Step 1'!$E$7</f>
+        <f>'[5]Step 1'!$E$7</f>
         <v>Ulta Beauty</v>
       </c>
       <c r="C2" t="s">
@@ -5662,11 +5872,11 @@
         <v>8100000000</v>
       </c>
       <c r="E5" s="13" t="str">
-        <f>'[3]Step 1'!$E$8</f>
+        <f>'[5]Step 1'!$E$8</f>
         <v>ULTA</v>
       </c>
       <c r="F5" s="13" t="str">
-        <f>'[3]XS Rating Step A Inputs'!$B$16</f>
+        <f>'[5]XS Rating Step A Inputs'!$B$16</f>
         <v>Public Organizations</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -5699,159 +5909,159 @@
         <v>101</v>
       </c>
       <c r="B6" s="15">
-        <f>'[3]Step 1'!$E$32</f>
+        <f>'[5]Step 1'!$E$32</f>
         <v>1</v>
       </c>
       <c r="C6" s="15">
-        <f>'[3]Step 1'!$E$33</f>
+        <f>'[5]Step 1'!$E$33</f>
         <v>1</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="15" cm="1">
-        <f t="array" ref="E6">INDEX('[3]Step 1'!$E$35:'[3]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$35:'[3]Step 1'!$E$37),0))</f>
-        <v>1</v>
+      <c r="E6" s="15" t="e" cm="1">
+        <f t="array" ref="E6">INDEX('[5]Step 1'!$E$35:'[5]Step 1'!$E$37, MATCH(FALSE, ISBLANK('[5]Step 1'!$E$35:'[5]Step 1'!$E$37),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="15" cm="1">
-        <f t="array" ref="G6">INDEX('[3]Step 1'!$E$39:'[3]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$39:'[3]Step 1'!$E$41),0))</f>
-        <v>1</v>
+      <c r="G6" s="15" t="e" cm="1">
+        <f t="array" ref="G6">INDEX('[5]Step 1'!$E$39:'[5]Step 1'!$E$41, MATCH(FALSE, ISBLANK('[5]Step 1'!$E$39:'[5]Step 1'!$E$41),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>244</v>
       </c>
       <c r="I6" s="15" cm="1">
-        <f t="array" ref="I6">INDEX('[3]Step 1'!$E$43:'[3]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$43:'[3]Step 1'!$E$44),0))</f>
+        <f t="array" ref="I6">INDEX('[5]Step 1'!$E$43:'[5]Step 1'!$E$44, MATCH(FALSE, ISBLANK('[5]Step 1'!$E$43:'[5]Step 1'!$E$44),0))</f>
         <v>1</v>
       </c>
       <c r="J6" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="15" cm="1">
-        <f t="array" ref="K6">INDEX('[3]Step 1'!$E$46:'[3]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$46:'[3]Step 1'!$E$48),0))</f>
-        <v>0.8</v>
+      <c r="K6" s="15" t="e" cm="1">
+        <f t="array" ref="K6">INDEX('[5]Step 1'!$E$46:'[5]Step 1'!$E$48, MATCH(FALSE, ISBLANK('[5]Step 1'!$E$46:'[5]Step 1'!$E$48),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="L6" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="M6" s="15" cm="1">
-        <f t="array" ref="M6">INDEX('[3]Step 1'!$E$50:'[3]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$50:'[3]Step 1'!$E$52),0))</f>
-        <v>1</v>
+      <c r="M6" s="15" t="e" cm="1">
+        <f t="array" ref="M6">INDEX('[5]Step 1'!$E$50:'[5]Step 1'!$E$52, MATCH(FALSE, ISBLANK('[5]Step 1'!$E$50:'[5]Step 1'!$E$52),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="N6" s="15">
-        <f>'[3]Step 1'!$E$54</f>
+        <f>'[5]Step 1'!$E$54</f>
         <v>1</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="P6" s="15" cm="1">
-        <f t="array" ref="P6">INDEX('[3]Step 1'!$E$56:'[3]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$56:'[3]Step 1'!$E$66),0))</f>
-        <v>1</v>
+      <c r="P6" s="15" t="e" cm="1">
+        <f t="array" ref="P6">INDEX('[5]Step 1'!$E$56:'[5]Step 1'!$E$66, MATCH(FALSE, ISBLANK('[5]Step 1'!$E$56:'[5]Step 1'!$E$66),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="Q6" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="R6" s="15" cm="1">
-        <f t="array" ref="R6">INDEX('[3]Step 1'!$E$69:'[3]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$69:'[3]Step 1'!$E$75),0))</f>
-        <v>0.9</v>
+      <c r="R6" s="15" t="e" cm="1">
+        <f t="array" ref="R6">INDEX('[5]Step 1'!$E$69:'[5]Step 1'!$E$75, MATCH(FALSE, ISBLANK('[5]Step 1'!$E$69:'[5]Step 1'!$E$75),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="S6" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="T6" s="15" cm="1">
-        <f t="array" ref="T6">INDEX('[3]Step 1'!$E$77:'[3]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[3]Step 1'!$E$77:'[3]Step 1'!$E$79),0))</f>
-        <v>2</v>
+      <c r="T6" s="15" t="e" cm="1">
+        <f t="array" ref="T6">INDEX('[5]Step 1'!$E$77:'[5]Step 1'!$E$79, MATCH(FALSE, ISBLANK('[5]Step 1'!$E$77:'[5]Step 1'!$E$79),0))</f>
+        <v>#REF!</v>
       </c>
       <c r="U6" s="15">
-        <f>'[3]Step 1'!$E$81</f>
+        <f>'[5]Step 1'!$E$81</f>
         <v>0.8</v>
       </c>
       <c r="V6" s="15">
-        <f>'[3]Step 1'!$E$82</f>
+        <f>'[5]Step 1'!$E$82</f>
         <v>0.9</v>
       </c>
       <c r="W6" s="15">
-        <f>'[3]Step 1'!$E$83</f>
+        <f>'[5]Step 1'!$E$83</f>
         <v>1</v>
       </c>
       <c r="X6" s="15">
-        <f>'[3]Step 1'!$E$84</f>
+        <f>'[5]Step 1'!$E$84</f>
         <v>0.95</v>
       </c>
       <c r="Y6" s="15">
-        <f>'[3]Step 1'!$E$85</f>
+        <f>'[5]Step 1'!$E$85</f>
         <v>1.45</v>
       </c>
       <c r="Z6" s="15">
-        <f>'[3]Step 1'!$E$86</f>
+        <f>'[5]Step 1'!$E$86</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AA6" s="15">
-        <f>'[3]Step 1'!$E$87</f>
+        <f>'[5]Step 1'!$E$87</f>
         <v>1.26</v>
       </c>
       <c r="AB6" s="15">
-        <f>'[3]Step 1'!$E$88</f>
+        <f>'[5]Step 1'!$E$88</f>
         <v>1</v>
       </c>
       <c r="AC6" s="15">
-        <f>'[3]Step 1'!$E$89</f>
+        <f>'[5]Step 1'!$E$89</f>
         <v>1</v>
       </c>
       <c r="AD6" s="15">
-        <f>'[3]Step 1'!$E$90</f>
+        <f>'[5]Step 1'!$E$90</f>
         <v>0.95</v>
       </c>
       <c r="AE6" s="15">
-        <f>'[3]Step 1'!$E$91</f>
+        <f>'[5]Step 1'!$E$91</f>
         <v>0.95</v>
       </c>
       <c r="AF6" s="15">
-        <f>'[3]Step 1'!$E$92</f>
+        <f>'[5]Step 1'!$E$92</f>
         <v>0.9</v>
       </c>
       <c r="AG6" s="15">
-        <f>'[3]Step 1'!$E$93</f>
+        <f>'[5]Step 1'!$E$93</f>
         <v>1</v>
       </c>
       <c r="AH6" s="15">
-        <f>'[3]Step 1'!$E$94</f>
+        <f>'[5]Step 1'!$E$94</f>
         <v>1</v>
       </c>
       <c r="AI6" s="15">
-        <f>'[3]Step 1'!$E$95</f>
+        <f>'[5]Step 1'!$E$95</f>
         <v>1</v>
       </c>
       <c r="AJ6" s="15">
-        <f>'[3]Step 1'!$E$96</f>
+        <f>'[5]Step 1'!$E$96</f>
         <v>1</v>
       </c>
       <c r="AK6" s="15">
-        <f>'[3]Step 1'!$E$97</f>
+        <f>'[5]Step 1'!$E$97</f>
         <v>1</v>
       </c>
       <c r="AL6" s="15">
-        <f>'[3]Step 1'!$E$98</f>
+        <f>'[5]Step 1'!$E$98</f>
         <v>1</v>
       </c>
       <c r="AM6" s="15">
-        <f>'[3]Step 1'!$E$99</f>
+        <f>'[5]Step 1'!$E$99</f>
         <v>0.95</v>
       </c>
       <c r="AN6" s="15">
-        <f>'[3]Step 1'!$E$100</f>
+        <f>'[5]Step 1'!$E$100</f>
         <v>1</v>
       </c>
       <c r="AO6" s="15">
-        <f>'[3]Step 1'!$E$101</f>
+        <f>'[5]Step 1'!$E$101</f>
         <v>1</v>
       </c>
       <c r="AP6" s="15">
-        <f>'[3]Step 1'!$E$102</f>
+        <f>'[5]Step 1'!$E$102</f>
         <v>1</v>
       </c>
     </row>
@@ -5952,15 +6162,15 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <f>'[3]Step 1'!$E$9</f>
+        <f>'[5]Step 1'!$E$9</f>
         <v>19500</v>
       </c>
       <c r="C18" s="11">
-        <f>'[3]Step 1'!$E$10</f>
+        <f>'[5]Step 1'!$E$10</f>
         <v>5100</v>
       </c>
       <c r="D18" s="11">
-        <f>'[3]Step 1'!$E$11</f>
+        <f>'[5]Step 1'!$E$11</f>
         <v>8100</v>
       </c>
     </row>
@@ -6319,11 +6529,11 @@
         <v>18</v>
       </c>
       <c r="E8">
-        <f>'[5]XS Rating Step A Inputs'!$A$20</f>
+        <f>'[6]XS Rating Step A Inputs'!$A$20</f>
         <v>1</v>
       </c>
       <c r="F8" t="str">
-        <f>'[5]XS Rating Step A Inputs'!$A$21</f>
+        <f>'[6]XS Rating Step A Inputs'!$A$21</f>
         <v>Low Risk</v>
       </c>
       <c r="G8" s="14" t="str">
@@ -6348,11 +6558,11 @@
         <v>18</v>
       </c>
       <c r="E9">
-        <f>'[5]XS Rating Step A Inputs'!$B$20</f>
+        <f>'[6]XS Rating Step A Inputs'!$B$20</f>
         <v>2</v>
       </c>
       <c r="F9" t="str">
-        <f>'[5]XS Rating Step A Inputs'!$B$21</f>
+        <f>'[6]XS Rating Step A Inputs'!$B$21</f>
         <v>Low/Medium Risk</v>
       </c>
       <c r="G9" s="14" t="str">
@@ -6377,11 +6587,11 @@
         <v>18</v>
       </c>
       <c r="E10">
-        <f>'[5]XS Rating Step A Inputs'!$C$20</f>
+        <f>'[6]XS Rating Step A Inputs'!$C$20</f>
         <v>3</v>
       </c>
       <c r="F10" t="str">
-        <f>'[5]XS Rating Step A Inputs'!$C$21</f>
+        <f>'[6]XS Rating Step A Inputs'!$C$21</f>
         <v>Medium Risk</v>
       </c>
       <c r="G10" s="14" t="str">
@@ -6406,11 +6616,11 @@
         <v>18</v>
       </c>
       <c r="E11">
-        <f>'[5]XS Rating Step A Inputs'!$D$20</f>
+        <f>'[6]XS Rating Step A Inputs'!$D$20</f>
         <v>4</v>
       </c>
       <c r="F11" t="str">
-        <f>'[5]XS Rating Step A Inputs'!$D$21</f>
+        <f>'[6]XS Rating Step A Inputs'!$D$21</f>
         <v>Medium/High Risk</v>
       </c>
       <c r="G11" s="14" t="str">
@@ -6435,11 +6645,11 @@
         <v>18</v>
       </c>
       <c r="E12">
-        <f>'[5]XS Rating Step A Inputs'!$E$20</f>
+        <f>'[6]XS Rating Step A Inputs'!$E$20</f>
         <v>5</v>
       </c>
       <c r="F12" t="str">
-        <f>'[5]XS Rating Step A Inputs'!$E$21</f>
+        <f>'[6]XS Rating Step A Inputs'!$E$21</f>
         <v>High Risk</v>
       </c>
       <c r="G12" s="14" t="str">
@@ -6521,7 +6731,7 @@
         <v>110</v>
       </c>
       <c r="H16" t="str">
-        <f>'[5]Step 1'!$B$39</f>
+        <f>'[6]Step 1'!$B$39</f>
         <v>Significant M&amp;A Activity /Level of M&amp;A Concern</v>
       </c>
       <c r="O16" s="32" t="s">
@@ -6542,11 +6752,11 @@
         <v>18</v>
       </c>
       <c r="F17" t="str">
-        <f>'[5]Step 1'!$C$39</f>
+        <f>'[6]Step 1'!$C$39</f>
         <v>Activity within 1 year / Very high concern</v>
       </c>
       <c r="G17" t="str">
-        <f>'[5]Step 1'!$D$39</f>
+        <f>'[6]Step 1'!$D$39</f>
         <v>1.30-1.50</v>
       </c>
       <c r="H17" s="17" t="str">
@@ -6571,11 +6781,11 @@
         <v>18</v>
       </c>
       <c r="F18" t="str">
-        <f>'[5]Step 1'!$C$40</f>
+        <f>'[6]Step 1'!$C$40</f>
         <v>Activity within 1-3 years / Material-high high concern</v>
       </c>
       <c r="G18" t="str">
-        <f>'[5]Step 1'!$D$40</f>
+        <f>'[6]Step 1'!$D$40</f>
         <v>1.20-1.30</v>
       </c>
       <c r="H18" s="17" t="str">
@@ -6600,11 +6810,11 @@
         <v>18</v>
       </c>
       <c r="F19" t="str">
-        <f>'[5]Step 1'!$C$41</f>
+        <f>'[6]Step 1'!$C$41</f>
         <v>No activity in last 3 years / Low or no concern</v>
       </c>
       <c r="G19" t="str">
-        <f>'[5]Step 1'!$D$41</f>
+        <f>'[6]Step 1'!$D$41</f>
         <v>0.80-1.20</v>
       </c>
       <c r="H19" s="17" t="str">
@@ -6652,7 +6862,7 @@
         <v>110</v>
       </c>
       <c r="H21" t="str">
-        <f>'[5]Step 1'!$B$35</f>
+        <f>'[6]Step 1'!$B$35</f>
         <v>Number of Years in Operation</v>
       </c>
     </row>
@@ -6667,11 +6877,11 @@
         <v>18</v>
       </c>
       <c r="F22" t="str">
-        <f>'[5]Step 1'!$C$35</f>
+        <f>'[6]Step 1'!$C$35</f>
         <v>&lt; 3 years</v>
       </c>
       <c r="G22" t="str">
-        <f>'[5]Step 1'!$D$35</f>
+        <f>'[6]Step 1'!$D$35</f>
         <v>1.05-1.25</v>
       </c>
       <c r="H22" s="16" t="str">
@@ -6690,11 +6900,11 @@
         <v>18</v>
       </c>
       <c r="F23" s="23" t="str">
-        <f>'[5]Step 1'!$C$36</f>
+        <f>'[6]Step 1'!$C$36</f>
         <v>=&lt;3 years and &lt;5 years</v>
       </c>
       <c r="G23" t="str">
-        <f>'[5]Step 1'!$D$36</f>
+        <f>'[6]Step 1'!$D$36</f>
         <v>1.00-1.05</v>
       </c>
       <c r="H23" s="16" t="str">
@@ -6713,11 +6923,11 @@
         <v>18</v>
       </c>
       <c r="F24" t="str">
-        <f>'[5]Step 1'!$C$37</f>
+        <f>'[6]Step 1'!$C$37</f>
         <v>&gt;5 years</v>
       </c>
       <c r="G24" t="str">
-        <f>'[5]Step 1'!$D$37</f>
+        <f>'[6]Step 1'!$D$37</f>
         <v>0.85-1.00</v>
       </c>
       <c r="H24" s="16" t="str">
@@ -6765,7 +6975,7 @@
         <v>110</v>
       </c>
       <c r="H26" t="str">
-        <f>'[5]Step 1'!$B$43</f>
+        <f>'[6]Step 1'!$B$43</f>
         <v>SEC Offering</v>
       </c>
       <c r="O26" s="36" t="s">
@@ -6786,11 +6996,11 @@
         <v>20</v>
       </c>
       <c r="F27" t="str">
-        <f>'[5]Step 1'!$C$43</f>
+        <f>'[6]Step 1'!$C$43</f>
         <v>Within 1 year</v>
       </c>
       <c r="G27" t="str">
-        <f>'[5]Step 1'!$D$43</f>
+        <f>'[6]Step 1'!$D$43</f>
         <v>1.00-1.55</v>
       </c>
       <c r="H27" s="18" t="str">
@@ -6815,11 +7025,11 @@
         <v>18</v>
       </c>
       <c r="F28" t="str">
-        <f>'[5]Step 1'!$C$44</f>
+        <f>'[6]Step 1'!$C$44</f>
         <v>None within last 12 months</v>
       </c>
       <c r="G28" t="str">
-        <f>'[5]Step 1'!$D$44</f>
+        <f>'[6]Step 1'!$D$44</f>
         <v>0.90-1.20</v>
       </c>
       <c r="H28" s="18" t="str">
@@ -6862,7 +7072,7 @@
         <v>110</v>
       </c>
       <c r="H30" t="str">
-        <f>'[5]Step 1'!$B$46</f>
+        <f>'[6]Step 1'!$B$46</f>
         <v>D&amp;O Litigation</v>
       </c>
       <c r="O30" s="38" t="s">
@@ -6883,11 +7093,11 @@
         <v>18</v>
       </c>
       <c r="F31" t="str">
-        <f>'[5]Step 1'!$C$46</f>
+        <f>'[6]Step 1'!$C$46</f>
         <v>Within 1 year</v>
       </c>
       <c r="G31" t="str">
-        <f>'[5]Step 1'!$D$46</f>
+        <f>'[6]Step 1'!$D$46</f>
         <v>1.20-1.50</v>
       </c>
       <c r="H31" s="19" t="str">
@@ -6912,11 +7122,11 @@
         <v>18</v>
       </c>
       <c r="F32" t="str">
-        <f>'[5]Step 1'!$C$47</f>
+        <f>'[6]Step 1'!$C$47</f>
         <v>Within 1-5 years</v>
       </c>
       <c r="G32" t="str">
-        <f>'[5]Step 1'!$D$47</f>
+        <f>'[6]Step 1'!$D$47</f>
         <v>1.00-1.50</v>
       </c>
       <c r="H32" s="19" t="str">
@@ -6941,11 +7151,11 @@
         <v>18</v>
       </c>
       <c r="F33" t="str">
-        <f>'[5]Step 1'!$C$48</f>
+        <f>'[6]Step 1'!$C$48</f>
         <v>Within 5-10 years</v>
       </c>
       <c r="G33" t="str">
-        <f>'[5]Step 1'!$D$48</f>
+        <f>'[6]Step 1'!$D$48</f>
         <v>0.80-1.10</v>
       </c>
       <c r="H33" s="19" t="str">
@@ -6993,7 +7203,7 @@
         <v>110</v>
       </c>
       <c r="H35" t="str">
-        <f>'[5]Step 1'!$B$50</f>
+        <f>'[6]Step 1'!$B$50</f>
         <v>Other Litigation</v>
       </c>
       <c r="O35" s="39" t="s">
@@ -7014,11 +7224,11 @@
         <v>18</v>
       </c>
       <c r="F36" t="str">
-        <f>'[5]Step 1'!$C$50</f>
+        <f>'[6]Step 1'!$C$50</f>
         <v>Potential Cost &gt;3% of assets</v>
       </c>
       <c r="G36" t="str">
-        <f>'[5]Step 1'!$D$50</f>
+        <f>'[6]Step 1'!$D$50</f>
         <v>1.20-1.30</v>
       </c>
       <c r="H36" s="20" t="str">
@@ -7037,11 +7247,11 @@
         <v>20</v>
       </c>
       <c r="F37" t="str">
-        <f>'[5]Step 1'!$C$51</f>
+        <f>'[6]Step 1'!$C$51</f>
         <v>Potential Cost 1-3% of assets</v>
       </c>
       <c r="G37" t="str">
-        <f>'[5]Step 1'!$D$51</f>
+        <f>'[6]Step 1'!$D$51</f>
         <v>1.10-1.20</v>
       </c>
       <c r="H37" s="20" t="str">
@@ -7060,11 +7270,11 @@
         <v>18</v>
       </c>
       <c r="F38" t="str">
-        <f>'[5]Step 1'!$C$52</f>
+        <f>'[6]Step 1'!$C$52</f>
         <v>Potential Cost &lt;1% of assets</v>
       </c>
       <c r="G38" t="str">
-        <f>'[5]Step 1'!$D$52</f>
+        <f>'[6]Step 1'!$D$52</f>
         <v>0.80-1.10</v>
       </c>
       <c r="H38" s="20" t="str">
@@ -7103,7 +7313,7 @@
         <v>110</v>
       </c>
       <c r="H40" t="str">
-        <f>'[5]Step 1'!$B$56</f>
+        <f>'[6]Step 1'!$B$56</f>
         <v>Coinsurance re SEC claims</v>
       </c>
       <c r="O40" s="40" t="s">
@@ -7121,11 +7331,11 @@
         <v>18</v>
       </c>
       <c r="F41" s="25">
-        <f>'[5]Step 1'!$C$56</f>
+        <f>'[6]Step 1'!$C$56</f>
         <v>0</v>
       </c>
       <c r="G41">
-        <f>'[5]Step 1'!$D$56</f>
+        <f>'[6]Step 1'!$D$56</f>
         <v>1</v>
       </c>
       <c r="H41" s="26" t="str">
@@ -7144,11 +7354,11 @@
         <v>18</v>
       </c>
       <c r="F42" s="25">
-        <f>'[5]Step 1'!$C$57</f>
+        <f>'[6]Step 1'!$C$57</f>
         <v>0.05</v>
       </c>
       <c r="G42" t="str">
-        <f>'[5]Step 1'!$D$57</f>
+        <f>'[6]Step 1'!$D$57</f>
         <v>0.95-0.97</v>
       </c>
       <c r="H42" s="26" t="str">
@@ -7170,11 +7380,11 @@
         <v>18</v>
       </c>
       <c r="F43" s="25">
-        <f>'[5]Step 1'!$C$58</f>
+        <f>'[6]Step 1'!$C$58</f>
         <v>0.1</v>
       </c>
       <c r="G43" t="str">
-        <f>'[5]Step 1'!$D$58</f>
+        <f>'[6]Step 1'!$D$58</f>
         <v>0.90-0.94</v>
       </c>
       <c r="H43" s="26" t="str">
@@ -7196,11 +7406,11 @@
         <v>18</v>
       </c>
       <c r="F44" s="25">
-        <f>'[5]Step 1'!$C$59</f>
+        <f>'[6]Step 1'!$C$59</f>
         <v>0.15</v>
       </c>
       <c r="G44" t="str">
-        <f>'[5]Step 1'!$D$59</f>
+        <f>'[6]Step 1'!$D$59</f>
         <v>0.87-0.91</v>
       </c>
       <c r="H44" s="26" t="str">
@@ -7222,11 +7432,11 @@
         <v>18</v>
       </c>
       <c r="F45" s="25">
-        <f>'[5]Step 1'!$C$60</f>
+        <f>'[6]Step 1'!$C$60</f>
         <v>0.2</v>
       </c>
       <c r="G45" t="str">
-        <f>'[5]Step 1'!$D$60</f>
+        <f>'[6]Step 1'!$D$60</f>
         <v>0.84-0.88</v>
       </c>
       <c r="H45" s="26" t="str">
@@ -7251,11 +7461,11 @@
         <v>111</v>
       </c>
       <c r="F46" s="25">
-        <f>'[5]Step 1'!$C$61</f>
+        <f>'[6]Step 1'!$C$61</f>
         <v>0.25</v>
       </c>
       <c r="G46" t="str">
-        <f>'[5]Step 1'!$D$61</f>
+        <f>'[6]Step 1'!$D$61</f>
         <v>0.81-0.85</v>
       </c>
       <c r="H46" s="26" t="str">
@@ -7281,11 +7491,11 @@
         <v>0%</v>
       </c>
       <c r="F47" s="25">
-        <f>'[5]Step 1'!$C$62</f>
+        <f>'[6]Step 1'!$C$62</f>
         <v>0.3</v>
       </c>
       <c r="G47" t="str">
-        <f>'[5]Step 1'!$D$62</f>
+        <f>'[6]Step 1'!$D$62</f>
         <v>0.78-0.82</v>
       </c>
       <c r="H47" s="26" t="str">
@@ -7311,11 +7521,11 @@
         <v>5%</v>
       </c>
       <c r="F48" s="25">
-        <f>'[5]Step 1'!$C$63</f>
+        <f>'[6]Step 1'!$C$63</f>
         <v>0.35</v>
       </c>
       <c r="G48" t="str">
-        <f>'[5]Step 1'!$D$63</f>
+        <f>'[6]Step 1'!$D$63</f>
         <v>0.75-0.79</v>
       </c>
       <c r="H48" s="26" t="str">
@@ -7338,11 +7548,11 @@
         <v>10%</v>
       </c>
       <c r="F49" s="25">
-        <f>'[5]Step 1'!$C$64</f>
+        <f>'[6]Step 1'!$C$64</f>
         <v>0.4</v>
       </c>
       <c r="G49" t="str">
-        <f>'[5]Step 1'!$D$64</f>
+        <f>'[6]Step 1'!$D$64</f>
         <v>0.72-0.76</v>
       </c>
       <c r="H49" s="26" t="str">
@@ -7365,11 +7575,11 @@
         <v>15%</v>
       </c>
       <c r="F50" s="25">
-        <f>'[5]Step 1'!$C$65</f>
+        <f>'[6]Step 1'!$C$65</f>
         <v>0.45</v>
       </c>
       <c r="G50" t="str">
-        <f>'[5]Step 1'!$D$65</f>
+        <f>'[6]Step 1'!$D$65</f>
         <v>0.70-0.74</v>
       </c>
       <c r="H50" s="26" t="str">
@@ -7395,11 +7605,11 @@
         <v>20%</v>
       </c>
       <c r="F51" s="25">
-        <f>'[5]Step 1'!$C$66</f>
+        <f>'[6]Step 1'!$C$66</f>
         <v>0.5</v>
       </c>
       <c r="G51" t="str">
-        <f>'[5]Step 1'!$D$66</f>
+        <f>'[6]Step 1'!$D$66</f>
         <v>0.68-0.72</v>
       </c>
       <c r="H51" s="26" t="str">
@@ -7440,7 +7650,7 @@
         <v>110</v>
       </c>
       <c r="H53" t="str">
-        <f>'[5]Step 1'!$B$69</f>
+        <f>'[6]Step 1'!$B$69</f>
         <v>Industry Risk/Level of Confidence in Industry</v>
       </c>
       <c r="O53" t="s">
@@ -7453,11 +7663,11 @@
         <v>35%</v>
       </c>
       <c r="F54" t="str">
-        <f>'[5]Step 1'!$C$69</f>
+        <f>'[6]Step 1'!$C$69</f>
         <v>Very Confident</v>
       </c>
       <c r="G54" t="str">
-        <f>'[5]Step 1'!$D$69</f>
+        <f>'[6]Step 1'!$D$69</f>
         <v>0.70-0.85</v>
       </c>
       <c r="H54" s="19" t="str">
@@ -7474,11 +7684,11 @@
         <v>40%</v>
       </c>
       <c r="F55" t="str">
-        <f>'[5]Step 1'!$C$70</f>
+        <f>'[6]Step 1'!$C$70</f>
         <v>Confident</v>
       </c>
       <c r="G55" t="str">
-        <f>'[5]Step 1'!$D$70</f>
+        <f>'[6]Step 1'!$D$70</f>
         <v>0.85-1.00</v>
       </c>
       <c r="H55" s="19" t="str">
@@ -7495,11 +7705,11 @@
         <v>45%</v>
       </c>
       <c r="F56" t="str">
-        <f>'[5]Step 1'!$C$71</f>
+        <f>'[6]Step 1'!$C$71</f>
         <v>Comfortable</v>
       </c>
       <c r="G56">
-        <f>'[5]Step 1'!$D$71</f>
+        <f>'[6]Step 1'!$D$71</f>
         <v>1</v>
       </c>
       <c r="H56" s="19" t="str">
@@ -7513,11 +7723,11 @@
         <v>50%</v>
       </c>
       <c r="F57" t="str">
-        <f>'[5]Step 1'!$C$72</f>
+        <f>'[6]Step 1'!$C$72</f>
         <v>Low Concern</v>
       </c>
       <c r="G57" t="str">
-        <f>'[5]Step 1'!$D$72</f>
+        <f>'[6]Step 1'!$D$72</f>
         <v>1.00-1.15</v>
       </c>
       <c r="H57" s="19" t="str">
@@ -7527,11 +7737,11 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F58" t="str">
-        <f>'[5]Step 1'!$C$73</f>
+        <f>'[6]Step 1'!$C$73</f>
         <v>Material Concern</v>
       </c>
       <c r="G58" t="str">
-        <f>'[5]Step 1'!$D$73</f>
+        <f>'[6]Step 1'!$D$73</f>
         <v>1.15-1.35</v>
       </c>
       <c r="H58" s="19" t="str">
@@ -7541,11 +7751,11 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F59" t="str">
-        <f>'[5]Step 1'!$C$74</f>
+        <f>'[6]Step 1'!$C$74</f>
         <v>High Concern</v>
       </c>
       <c r="G59" t="str">
-        <f>'[5]Step 1'!$D$74</f>
+        <f>'[6]Step 1'!$D$74</f>
         <v>1.35-1.75</v>
       </c>
       <c r="H59" s="19" t="str">
@@ -7555,11 +7765,11 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F60" t="str">
-        <f>'[5]Step 1'!$C$75</f>
+        <f>'[6]Step 1'!$C$75</f>
         <v>Very High to Severe Concern</v>
       </c>
       <c r="G60" t="str">
-        <f>'[5]Step 1'!$D$75</f>
+        <f>'[6]Step 1'!$D$75</f>
         <v>1.75-1.25</v>
       </c>
       <c r="H60" s="19" t="str">
@@ -7575,17 +7785,17 @@
         <v>110</v>
       </c>
       <c r="H62" t="str">
-        <f>'[5]Step 1'!$B$77</f>
+        <f>'[6]Step 1'!$B$77</f>
         <v>Discovery (Extended Reporting)</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F63" t="str">
-        <f>'[5]Step 1'!$C$77</f>
+        <f>'[6]Step 1'!$C$77</f>
         <v>1 year</v>
       </c>
       <c r="G63">
-        <f>'[4]Step 1'!$D$77</f>
+        <f>'[3]Step 1'!$D$77</f>
         <v>1</v>
       </c>
       <c r="H63" s="22" t="str">
@@ -7595,11 +7805,11 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F64" t="str">
-        <f>'[5]Step 1'!$C$78</f>
+        <f>'[6]Step 1'!$C$78</f>
         <v>2 years</v>
       </c>
       <c r="G64" t="str">
-        <f>'[4]Step 1'!$D$78</f>
+        <f>'[3]Step 1'!$D$78</f>
         <v>1.75-2.00</v>
       </c>
       <c r="H64" s="22" t="str">
@@ -7609,11 +7819,11 @@
     </row>
     <row r="65" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F65" t="str">
-        <f>'[5]Step 1'!$C$79</f>
+        <f>'[6]Step 1'!$C$79</f>
         <v>3 years</v>
       </c>
       <c r="G65" t="str">
-        <f>'[4]Step 1'!$D$79</f>
+        <f>'[3]Step 1'!$D$79</f>
         <v>2.25-2.50</v>
       </c>
       <c r="H65" s="22" t="str">

</xml_diff>